<commit_message>
fixing seeds: now  uses  context
</commit_message>
<xml_diff>
--- a/seeds/seeds.xlsx
+++ b/seeds/seeds.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="357">
   <si>
     <t>id</t>
   </si>
@@ -701,6 +701,9 @@
     <t>id_type</t>
   </si>
   <si>
+    <t>address</t>
+  </si>
+  <si>
     <t>id_sponsor</t>
   </si>
   <si>
@@ -710,202 +713,283 @@
     <t>Cinelândia</t>
   </si>
   <si>
+    <t>Rua Dos Filmes, 324</t>
+  </si>
+  <si>
     <t>uuid-restaurante-da-rose</t>
   </si>
   <si>
     <t>Restaurante da Rose</t>
   </si>
   <si>
+    <t>Avenida dos Pratos, 123</t>
+  </si>
+  <si>
     <t>uuid-parquemania</t>
   </si>
   <si>
     <t>Parquemania</t>
   </si>
   <si>
+    <t>Rua da Alegria, 123</t>
+  </si>
+  <si>
     <t>uuid-parque-da-crianca</t>
   </si>
   <si>
     <t>Parque da Criança</t>
   </si>
   <si>
+    <t>Rua Central, 32</t>
+  </si>
+  <si>
     <t>uuid-museu-do-espaco</t>
   </si>
   <si>
     <t>Museu do espaço</t>
   </si>
   <si>
+    <t>Avenida da descoberta, 123</t>
+  </si>
+  <si>
     <t>uuid-teatro-rural</t>
   </si>
   <si>
     <t>Teatro Rural</t>
   </si>
   <si>
+    <t>Rua dos Bois, 23</t>
+  </si>
+  <si>
     <t>uuid-zoo-safari-a-dentro</t>
   </si>
   <si>
     <t>Zoo Safari a Dentro</t>
   </si>
   <si>
+    <t>Avenida da Selva, 32</t>
+  </si>
+  <si>
     <t>uuid-lagoa-azul</t>
   </si>
   <si>
     <t>Lagoa Azul</t>
   </si>
   <si>
+    <t>Rua da Criança, 43</t>
+  </si>
+  <si>
     <t>uuid-serra-dos-cavalos</t>
   </si>
   <si>
     <t>Serra dos Cavalos</t>
   </si>
   <si>
+    <t>Trila ecológica do cavalo</t>
+  </si>
+  <si>
     <t>uuid-veneza-parque</t>
   </si>
   <si>
     <t>Veneza Parque</t>
   </si>
   <si>
+    <t>Rodovia das Águas, km 34</t>
+  </si>
+  <si>
     <t>uuid-centro-de-descobertas</t>
   </si>
   <si>
     <t>Centro de descobertas</t>
   </si>
   <si>
+    <t>Rua da descoberta, 32</t>
+  </si>
+  <si>
     <t>uuid-museu-das-artes</t>
   </si>
   <si>
     <t>Museu das Artes</t>
   </si>
   <si>
+    <t>Rua do Cateiro, 211</t>
+  </si>
+  <si>
     <t>uuid-jardim-botanico-da-cidade</t>
   </si>
   <si>
     <t>Jardim Botanico da Cidade</t>
   </si>
   <si>
+    <t>Rodovia Luiz Gonzaga, 43</t>
+  </si>
+  <si>
+    <t>uuid-patinaco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patinaço </t>
+  </si>
+  <si>
+    <t>Shopping da Cidade, 12</t>
+  </si>
+  <si>
+    <t>uuid-fliperama</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fliperama </t>
+  </si>
+  <si>
+    <t>Avenida dos Jogos, 34</t>
+  </si>
+  <si>
+    <t>uuid-museu-da-criaca</t>
+  </si>
+  <si>
+    <t>Museu da Criaça</t>
+  </si>
+  <si>
+    <t>Rua da história, 11</t>
+  </si>
+  <si>
+    <t>uuid-picinic-da-sol</t>
+  </si>
+  <si>
+    <t>Picinic da Sol</t>
+  </si>
+  <si>
+    <t>Praça da Iluminação, centro</t>
+  </si>
+  <si>
+    <t>uuid-baoba</t>
+  </si>
+  <si>
+    <t>Baobá</t>
+  </si>
+  <si>
+    <t>Rua da  Selva, 42</t>
+  </si>
+  <si>
+    <t>uuid-rancho-alegre</t>
+  </si>
+  <si>
+    <t>Rancho Alegre</t>
+  </si>
+  <si>
+    <t>Avenida do Rancho, 235</t>
+  </si>
+  <si>
+    <t>uuid-piscinao-azul</t>
+  </si>
+  <si>
+    <t>Piscinão Azul</t>
+  </si>
+  <si>
+    <t>Rua dos clubes, 32</t>
+  </si>
+  <si>
+    <t>uuid-burguelandia</t>
+  </si>
+  <si>
+    <t>Burguelândia</t>
+  </si>
+  <si>
+    <t>Rua das comidas, 43</t>
+  </si>
+  <si>
+    <t>uuid-pizzamania</t>
+  </si>
+  <si>
+    <t>Pizzamania</t>
+  </si>
+  <si>
+    <t>uuid-casa-club</t>
+  </si>
+  <si>
+    <t>Casa Club</t>
+  </si>
+  <si>
+    <t>Rua dos clubes, 45</t>
+  </si>
+  <si>
+    <t>review</t>
+  </si>
+  <si>
+    <t>stars</t>
+  </si>
+  <si>
+    <t>id_user</t>
+  </si>
+  <si>
+    <t>Um lugar incrível para os amantes de cinema! A qualidade do som e da imagem é excelente, e a seleção de filmes sempre inclui os últimos lançamentos.</t>
+  </si>
+  <si>
+    <t>Comida caseira autêntica e um ambiente acolhedor. A Rose faz você se sentir em casa. Não deixe de provar o estrogonofe!</t>
+  </si>
+  <si>
+    <t>Um parque de diversões que superou todas as nossas expectativas! Ideal para todas as idades, com muitas atrações radicais e áreas temáticas.</t>
+  </si>
+  <si>
+    <t>Perfeito para um dia em família! Muitas atividades interativas para as crianças e espaços de descanso para os adultos</t>
+  </si>
+  <si>
+    <t>Fascinante! A exposição interativa é uma jornada incrível pelo universo. Recomendo muito para quem tem interesse em astronomia</t>
+  </si>
+  <si>
+    <t>Uma experiência única que combina arte e natureza. As peças são sempre emocionantes e o cenário ao ar livre é deslumbrante.</t>
+  </si>
+  <si>
+    <t>Uma experiência inesquecível! Ver os animais tão de perto foi emocionante. Excelente programa para as crianças aprenderem sobre conservação.</t>
+  </si>
+  <si>
+    <t>Um oásis de tranquilidade. Águas cristalinas e perfeitas para um mergulho refrescante. Um lugar maravilhoso para relaxar e se conectar com a natureza.</t>
+  </si>
+  <si>
+    <t>Para os aventureiros de plantão, a Serra dos Cavalos oferece trilhas desafiadoras com vistas de tirar o fôlego. Vale cada passo!</t>
+  </si>
+  <si>
+    <t>Uma mini-Veneza que encanta a todos. Os passeios de gôndola são românticos e a arquitetura é impressionante. Um pedacinho da Itália na cidade</t>
+  </si>
+  <si>
+    <t>Interativo e educativo, é o lugar ideal para crianças curiosas. As exposições mudam frequentemente, sempre trazendo novidades</t>
+  </si>
+  <si>
+    <t>Um espaço sublime que abriga coleções de arte impressionantes. A cada visita, descubro algo novo. Uma jóia cultural.</t>
+  </si>
+  <si>
+    <t>Um refúgio verde no meio da cidade. A diversidade de plantas e flores é estonteante, e os caminhos são perfeitos para uma caminhada tranquila.</t>
+  </si>
+  <si>
     <t>uuid-patinaço</t>
   </si>
   <si>
-    <t xml:space="preserve">Patinaço </t>
-  </si>
-  <si>
-    <t>uuid-fliperama</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fliperama </t>
-  </si>
-  <si>
-    <t>uuid-museu-da-criaca</t>
-  </si>
-  <si>
-    <t>Museu da Criaça</t>
-  </si>
-  <si>
-    <t>uuid-picinic-da-sol</t>
-  </si>
-  <si>
-    <t>Picinic da Sol</t>
-  </si>
-  <si>
-    <t>uuid-baoba</t>
-  </si>
-  <si>
-    <t>Baobá</t>
-  </si>
-  <si>
-    <t>uuid-rancho-alegre</t>
-  </si>
-  <si>
-    <t>Rancho Alegre</t>
+    <t>A pista de patinação é ampla e bem cuidada. Um lugar divertido para famílias e amigos. Eles também oferecem aulas para iniciantes</t>
+  </si>
+  <si>
+    <t>Voltar no tempo e reviver a infância. O fliperama tem uma ótima seleção de jogos clássicos e novos. Ótimo lugar para se divertir.</t>
+  </si>
+  <si>
+    <t>Um lugar mágico cheio de atividades lúdicas e educativas. Meus filhos amaram e aprenderam muito brincando.</t>
+  </si>
+  <si>
+    <t>O local perfeito para um piquenique em família ou com amigos. Muita grama verde, sombras agradáveis e uma vista deslumbrante do pôr do sol.</t>
+  </si>
+  <si>
+    <t>Visitar o Baobá é como entrar em um conto de fadas. A árvore é majestosa e o ambiente ao redor é pacífico. Uma experiência memorável.</t>
+  </si>
+  <si>
+    <t>Um dia no campo cheio de diversão e aprendizado. As atividades de fazenda são ótimas para as crianças, e os funcionários são super simpáticos.</t>
   </si>
   <si>
     <t>uuid-piscinão-azul</t>
   </si>
   <si>
-    <t>Piscinão Azul</t>
-  </si>
-  <si>
-    <t>uuid-burguelandia</t>
-  </si>
-  <si>
-    <t>Burguelândia</t>
+    <t>A melhor fuga do calor! O parque aquático tem opções para todos, desde piscinas tranquilas até escorregadores emocionantes.</t>
+  </si>
+  <si>
+    <t>O paraíso dos hambúrgueres! Cada opção no menu é mais deliciosa que a outra. O ambiente é descontraído e perfeito para encontros</t>
   </si>
   <si>
     <t>uuid-pizzarolla</t>
-  </si>
-  <si>
-    <t>Pizzarolla</t>
-  </si>
-  <si>
-    <t>review</t>
-  </si>
-  <si>
-    <t>stars</t>
-  </si>
-  <si>
-    <t>id_user</t>
-  </si>
-  <si>
-    <t>Um lugar incrível para os amantes de cinema! A qualidade do som e da imagem é excelente, e a seleção de filmes sempre inclui os últimos lançamentos.</t>
-  </si>
-  <si>
-    <t>Comida caseira autêntica e um ambiente acolhedor. A Rose faz você se sentir em casa. Não deixe de provar o estrogonofe!</t>
-  </si>
-  <si>
-    <t>Um parque de diversões que superou todas as nossas expectativas! Ideal para todas as idades, com muitas atrações radicais e áreas temáticas.</t>
-  </si>
-  <si>
-    <t>Perfeito para um dia em família! Muitas atividades interativas para as crianças e espaços de descanso para os adultos</t>
-  </si>
-  <si>
-    <t>Fascinante! A exposição interativa é uma jornada incrível pelo universo. Recomendo muito para quem tem interesse em astronomia</t>
-  </si>
-  <si>
-    <t>Uma experiência única que combina arte e natureza. As peças são sempre emocionantes e o cenário ao ar livre é deslumbrante.</t>
-  </si>
-  <si>
-    <t>Uma experiência inesquecível! Ver os animais tão de perto foi emocionante. Excelente programa para as crianças aprenderem sobre conservação.</t>
-  </si>
-  <si>
-    <t>Um oásis de tranquilidade. Águas cristalinas e perfeitas para um mergulho refrescante. Um lugar maravilhoso para relaxar e se conectar com a natureza.</t>
-  </si>
-  <si>
-    <t>Para os aventureiros de plantão, a Serra dos Cavalos oferece trilhas desafiadoras com vistas de tirar o fôlego. Vale cada passo!</t>
-  </si>
-  <si>
-    <t>Uma mini-Veneza que encanta a todos. Os passeios de gôndola são românticos e a arquitetura é impressionante. Um pedacinho da Itália na cidade</t>
-  </si>
-  <si>
-    <t>Interativo e educativo, é o lugar ideal para crianças curiosas. As exposições mudam frequentemente, sempre trazendo novidades</t>
-  </si>
-  <si>
-    <t>Um espaço sublime que abriga coleções de arte impressionantes. A cada visita, descubro algo novo. Uma jóia cultural.</t>
-  </si>
-  <si>
-    <t>Um refúgio verde no meio da cidade. A diversidade de plantas e flores é estonteante, e os caminhos são perfeitos para uma caminhada tranquila.</t>
-  </si>
-  <si>
-    <t>A pista de patinação é ampla e bem cuidada. Um lugar divertido para famílias e amigos. Eles também oferecem aulas para iniciantes</t>
-  </si>
-  <si>
-    <t>Voltar no tempo e reviver a infância. O fliperama tem uma ótima seleção de jogos clássicos e novos. Ótimo lugar para se divertir.</t>
-  </si>
-  <si>
-    <t>Um lugar mágico cheio de atividades lúdicas e educativas. Meus filhos amaram e aprenderam muito brincando.</t>
-  </si>
-  <si>
-    <t>O local perfeito para um piquenique em família ou com amigos. Muita grama verde, sombras agradáveis e uma vista deslumbrante do pôr do sol.</t>
-  </si>
-  <si>
-    <t>Visitar o Baobá é como entrar em um conto de fadas. A árvore é majestosa e o ambiente ao redor é pacífico. Uma experiência memorável.</t>
-  </si>
-  <si>
-    <t>Um dia no campo cheio de diversão e aprendizado. As atividades de fazenda são ótimas para as crianças, e os funcionários são super simpáticos.</t>
-  </si>
-  <si>
-    <t>A melhor fuga do calor! O parque aquático tem opções para todos, desde piscinas tranquilas até escorregadores emocionantes.</t>
-  </si>
-  <si>
-    <t>O paraíso dos hambúrgueres! Cada opção no menu é mais deliciosa que a outra. O ambiente é descontraído e perfeito para encontros</t>
   </si>
   <si>
     <t>Uma pizzaria que se destaca. A massa fina e crocante e os ingredientes frescos fazem toda a diferença. Excelente atendimento também</t>
@@ -1473,6 +1557,10 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="G1" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("UNIQUE(A:A)"),"id")</f>
+        <v>id</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
@@ -1490,6 +1578,10 @@
       <c r="E2" s="3">
         <v>43834.125</v>
       </c>
+      <c r="G2" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-joey-doe")</f>
+        <v>uuid-joey-doe</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
@@ -1507,6 +1599,10 @@
       <c r="E3" s="3">
         <v>43835.125</v>
       </c>
+      <c r="G3" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-jane-silva")</f>
+        <v>uuid-jane-silva</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
@@ -1524,6 +1620,10 @@
       <c r="E4" s="3">
         <v>43875.125</v>
       </c>
+      <c r="G4" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-ivan-luiz")</f>
+        <v>uuid-ivan-luiz</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
@@ -1541,6 +1641,10 @@
       <c r="E5" s="3">
         <v>43837.125</v>
       </c>
+      <c r="G5" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-jose-maria")</f>
+        <v>uuid-jose-maria</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
@@ -1558,6 +1662,10 @@
       <c r="E6" s="3">
         <v>43875.125</v>
       </c>
+      <c r="G6" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-sandra-luna")</f>
+        <v>uuid-sandra-luna</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
@@ -1575,6 +1683,10 @@
       <c r="E7" s="3">
         <v>43895.125</v>
       </c>
+      <c r="G7" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-lucas-silva")</f>
+        <v>uuid-lucas-silva</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
@@ -1592,6 +1704,10 @@
       <c r="E8" s="3">
         <v>43859.125</v>
       </c>
+      <c r="G8" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-carla-almeida")</f>
+        <v>uuid-carla-almeida</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
@@ -1609,6 +1725,10 @@
       <c r="E9" s="3">
         <v>43924.125</v>
       </c>
+      <c r="G9" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-maria-julia")</f>
+        <v>uuid-maria-julia</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
@@ -1626,6 +1746,10 @@
       <c r="E10" s="3">
         <v>43834.125</v>
       </c>
+      <c r="G10" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-ana-paula")</f>
+        <v>uuid-ana-paula</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
@@ -1643,6 +1767,10 @@
       <c r="E11" s="3">
         <v>44932.125</v>
       </c>
+      <c r="G11" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-mario-neto")</f>
+        <v>uuid-mario-neto</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
@@ -1660,6 +1788,10 @@
       <c r="E12" s="3">
         <v>45349.125</v>
       </c>
+      <c r="G12" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-luiza-santos")</f>
+        <v>uuid-luiza-santos</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
@@ -1677,6 +1809,10 @@
       <c r="E13" s="3">
         <v>44973.125</v>
       </c>
+      <c r="G13" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-pedro-henrique")</f>
+        <v>uuid-pedro-henrique</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
@@ -1694,6 +1830,10 @@
       <c r="E14" s="3">
         <v>43904.125</v>
       </c>
+      <c r="G14" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-caroline-dias")</f>
+        <v>uuid-caroline-dias</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
@@ -1711,6 +1851,10 @@
       <c r="E15" s="3">
         <v>43856.125</v>
       </c>
+      <c r="G15" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-felipe-araujo")</f>
+        <v>uuid-felipe-araujo</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
@@ -1728,6 +1872,10 @@
       <c r="E16" s="3">
         <v>43855.125</v>
       </c>
+      <c r="G16" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-gabriela-moura")</f>
+        <v>uuid-gabriela-moura</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
@@ -1745,6 +1893,10 @@
       <c r="E17" s="3">
         <v>43886.125</v>
       </c>
+      <c r="G17" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-rodrigo-lima")</f>
+        <v>uuid-rodrigo-lima</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
@@ -1762,6 +1914,10 @@
       <c r="E18" s="3">
         <v>43866.125</v>
       </c>
+      <c r="G18" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-sophia-castro")</f>
+        <v>uuid-sophia-castro</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
@@ -1779,6 +1935,10 @@
       <c r="E19" s="3">
         <v>43888.125</v>
       </c>
+      <c r="G19" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-guilherme-oliveira")</f>
+        <v>uuid-guilherme-oliveira</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
@@ -1796,6 +1956,10 @@
       <c r="E20" s="3">
         <v>43852.125</v>
       </c>
+      <c r="G20" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-marcela-rodrigues")</f>
+        <v>uuid-marcela-rodrigues</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
@@ -1813,6 +1977,10 @@
       <c r="E21" s="3">
         <v>43887.125</v>
       </c>
+      <c r="G21" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-thiago-menezes")</f>
+        <v>uuid-thiago-menezes</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
@@ -1830,6 +1998,10 @@
       <c r="E22" s="3">
         <v>43946.125</v>
       </c>
+      <c r="G22" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-amanda-ferreira")</f>
+        <v>uuid-amanda-ferreira</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
@@ -1847,6 +2019,10 @@
       <c r="E23" s="3">
         <v>43852.125</v>
       </c>
+      <c r="G23" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-rafael-souza")</f>
+        <v>uuid-rafael-souza</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
@@ -1864,6 +2040,10 @@
       <c r="E24" s="3">
         <v>44962.125</v>
       </c>
+      <c r="G24" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-larissa-machado")</f>
+        <v>uuid-larissa-machado</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
@@ -1881,6 +2061,10 @@
       <c r="E25" s="3">
         <v>45349.125</v>
       </c>
+      <c r="G25" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-vinicius-costa")</f>
+        <v>uuid-vinicius-costa</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
@@ -1898,6 +2082,10 @@
       <c r="E26" s="3">
         <v>43839.125</v>
       </c>
+      <c r="G26" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-beatriz-lima")</f>
+        <v>uuid-beatriz-lima</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
@@ -1915,6 +2103,10 @@
       <c r="E27" s="3">
         <v>43886.125</v>
       </c>
+      <c r="G27" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-caio-martins")</f>
+        <v>uuid-caio-martins</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
@@ -1932,6 +2124,10 @@
       <c r="E28" s="3">
         <v>43910.125</v>
       </c>
+      <c r="G28" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-daniela-pires")</f>
+        <v>uuid-daniela-pires</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
@@ -1949,6 +2145,10 @@
       <c r="E29" s="3">
         <v>43859.125</v>
       </c>
+      <c r="G29" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-henrique-fonseca")</f>
+        <v>uuid-henrique-fonseca</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
@@ -1966,6 +2166,10 @@
       <c r="E30" s="3">
         <v>43861.125</v>
       </c>
+      <c r="G30" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-alice-barbosa")</f>
+        <v>uuid-alice-barbosa</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
@@ -1983,6 +2187,10 @@
       <c r="E31" s="3">
         <v>43899.125</v>
       </c>
+      <c r="G31" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-joão-victor")</f>
+        <v>uuid-joão-victor</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
@@ -2000,6 +2208,10 @@
       <c r="E32" s="3">
         <v>43865.125</v>
       </c>
+      <c r="G32" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-clara-nunes")</f>
+        <v>uuid-clara-nunes</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
@@ -2017,6 +2229,10 @@
       <c r="E33" s="3">
         <v>44981.125</v>
       </c>
+      <c r="G33" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-leonardo-teixeira")</f>
+        <v>uuid-leonardo-teixeira</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
@@ -2034,6 +2250,10 @@
       <c r="E34" s="3">
         <v>45295.125</v>
       </c>
+      <c r="G34" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-julia-vasconcelos")</f>
+        <v>uuid-julia-vasconcelos</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
@@ -2051,6 +2271,10 @@
       <c r="E35" s="3">
         <v>43844.125</v>
       </c>
+      <c r="G35" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-marcos-ribeiro")</f>
+        <v>uuid-marcos-ribeiro</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
@@ -2068,6 +2292,10 @@
       <c r="E36" s="3">
         <v>43837.125</v>
       </c>
+      <c r="G36" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-isabela-freitas")</f>
+        <v>uuid-isabela-freitas</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
@@ -2085,6 +2313,10 @@
       <c r="E37" s="3">
         <v>43919.125</v>
       </c>
+      <c r="G37" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-gustavo-pereira")</f>
+        <v>uuid-gustavo-pereira</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
@@ -2102,6 +2334,10 @@
       <c r="E38" s="3">
         <v>43897.125</v>
       </c>
+      <c r="G38" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-elisa-martinez")</f>
+        <v>uuid-elisa-martinez</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
@@ -2119,6 +2355,10 @@
       <c r="E39" s="3">
         <v>43893.125</v>
       </c>
+      <c r="G39" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-ricardo-alves")</f>
+        <v>uuid-ricardo-alves</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
@@ -2136,6 +2376,10 @@
       <c r="E40" s="3">
         <v>43876.125</v>
       </c>
+      <c r="G40" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-sara-carvalho")</f>
+        <v>uuid-sara-carvalho</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
@@ -2153,6 +2397,10 @@
       <c r="E41" s="3">
         <v>43937.125</v>
       </c>
+      <c r="G41" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-fernando-magalhães")</f>
+        <v>uuid-fernando-magalhães</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
@@ -2170,6 +2418,10 @@
       <c r="E42" s="3">
         <v>43907.125</v>
       </c>
+      <c r="G42" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-luana-borges")</f>
+        <v>uuid-luana-borges</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
@@ -2187,6 +2439,10 @@
       <c r="E43" s="3">
         <v>44982.125</v>
       </c>
+      <c r="G43" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-andre-luiz")</f>
+        <v>uuid-andre-luiz</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
@@ -2204,6 +2460,10 @@
       <c r="E44" s="3">
         <v>45360.125</v>
       </c>
+      <c r="G44" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-patricia-leal")</f>
+        <v>uuid-patricia-leal</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
@@ -2221,6 +2481,10 @@
       <c r="E45" s="3">
         <v>45373.125</v>
       </c>
+      <c r="G45" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-diego-santana")</f>
+        <v>uuid-diego-santana</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
@@ -2238,6 +2502,10 @@
       <c r="E46" s="3">
         <v>43930.125</v>
       </c>
+      <c r="G46" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-renata-melo")</f>
+        <v>uuid-renata-melo</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="s">
@@ -2255,6 +2523,10 @@
       <c r="E47" s="3">
         <v>43864.125</v>
       </c>
+      <c r="G47" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-cesar-augusto")</f>
+        <v>uuid-cesar-augusto</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
@@ -2272,6 +2544,10 @@
       <c r="E48" s="3">
         <v>43835.125</v>
       </c>
+      <c r="G48" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-monica-gomes")</f>
+        <v>uuid-monica-gomes</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="s">
@@ -2289,6 +2565,10 @@
       <c r="E49" s="3">
         <v>43836.125</v>
       </c>
+      <c r="G49" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-fabio-lopes")</f>
+        <v>uuid-fabio-lopes</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="s">
@@ -2306,6 +2586,10 @@
       <c r="E50" s="3">
         <v>43837.125</v>
       </c>
+      <c r="G50" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-anita-oliveira")</f>
+        <v>uuid-anita-oliveira</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="s">
@@ -2323,6 +2607,10 @@
       <c r="E51" s="3">
         <v>43838.125</v>
       </c>
+      <c r="G51" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-bruno-gonzalez")</f>
+        <v>uuid-bruno-gonzalez</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="s">
@@ -2340,6 +2628,10 @@
       <c r="E52" s="3">
         <v>43857.125</v>
       </c>
+      <c r="G52" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-carolina-queiroz")</f>
+        <v>uuid-carolina-queiroz</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="s">
@@ -2357,6 +2649,10 @@
       <c r="E53" s="3">
         <v>43861.125</v>
       </c>
+      <c r="G53" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-daniel-fernandes")</f>
+        <v>uuid-daniel-fernandes</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="s">
@@ -2374,6 +2670,10 @@
       <c r="E54" s="3">
         <v>43901.125</v>
       </c>
+      <c r="G54" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-ester-vieira")</f>
+        <v>uuid-ester-vieira</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="s">
@@ -2391,6 +2691,10 @@
       <c r="E55" s="3">
         <v>43842.125</v>
       </c>
+      <c r="G55" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-fabiana-mourão")</f>
+        <v>uuid-fabiana-mourão</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="s">
@@ -2408,6 +2712,10 @@
       <c r="E56" s="3">
         <v>44951.125</v>
       </c>
+      <c r="G56" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-gabriel-nascimento")</f>
+        <v>uuid-gabriel-nascimento</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="s">
@@ -2425,6 +2733,10 @@
       <c r="E57" s="3">
         <v>45337.125</v>
       </c>
+      <c r="G57" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-helena-ribeiro")</f>
+        <v>uuid-helena-ribeiro</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="s">
@@ -2442,6 +2754,10 @@
       <c r="E58" s="3">
         <v>43887.125</v>
       </c>
+      <c r="G58" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-igor-campos")</f>
+        <v>uuid-igor-campos</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="s">
@@ -2459,6 +2775,10 @@
       <c r="E59" s="3">
         <v>43898.125</v>
       </c>
+      <c r="G59" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-jessica-lima")</f>
+        <v>uuid-jessica-lima</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="s">
@@ -2476,6 +2796,10 @@
       <c r="E60" s="3">
         <v>43909.125</v>
       </c>
+      <c r="G60" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-kleber-martins")</f>
+        <v>uuid-kleber-martins</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="s">
@@ -2493,6 +2817,10 @@
       <c r="E61" s="3">
         <v>43920.125</v>
       </c>
+      <c r="G61" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-livia-souza")</f>
+        <v>uuid-livia-souza</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="s">
@@ -2510,6 +2838,10 @@
       <c r="E62" s="3">
         <v>43843.125</v>
       </c>
+      <c r="G62" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-marcelo-pinto")</f>
+        <v>uuid-marcelo-pinto</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="s">
@@ -2527,6 +2859,10 @@
       <c r="E63" s="3">
         <v>43854.125</v>
       </c>
+      <c r="G63" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-nadia-correia")</f>
+        <v>uuid-nadia-correia</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="s">
@@ -2544,6 +2880,10 @@
       <c r="E64" s="3">
         <v>43872.125</v>
       </c>
+      <c r="G64" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-oscar-neves")</f>
+        <v>uuid-oscar-neves</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="s">
@@ -2561,6 +2901,10 @@
       <c r="E65" s="3">
         <v>43864.125</v>
       </c>
+      <c r="G65" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-paula-rodrigues")</f>
+        <v>uuid-paula-rodrigues</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="s">
@@ -2578,6 +2922,10 @@
       <c r="E66" s="3">
         <v>43903.125</v>
       </c>
+      <c r="G66" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-quiteria-machado")</f>
+        <v>uuid-quiteria-machado</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="s">
@@ -2595,6 +2943,10 @@
       <c r="E67" s="3">
         <v>43853.125</v>
       </c>
+      <c r="G67" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-roberto-silveira")</f>
+        <v>uuid-roberto-silveira</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="s">
@@ -2612,6 +2964,10 @@
       <c r="E68" s="3">
         <v>44961.125</v>
       </c>
+      <c r="G68" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-silvia-penna")</f>
+        <v>uuid-silvia-penna</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="s">
@@ -2629,6 +2985,13 @@
       <c r="E69" s="3">
         <v>45304.125</v>
       </c>
+      <c r="G69" s="4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"uuid-tiago-lobo")</f>
+        <v>uuid-tiago-lobo</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="G70" s="4"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -2648,9 +3011,9 @@
     <col customWidth="1" min="1" max="1" width="23.38"/>
     <col customWidth="1" min="2" max="2" width="20.5"/>
     <col customWidth="1" min="3" max="3" width="27.0"/>
-    <col customWidth="1" min="4" max="4" width="18.38"/>
-    <col customWidth="1" min="5" max="5" width="20.38"/>
-    <col customWidth="1" min="6" max="6" width="17.0"/>
+    <col customWidth="1" min="4" max="5" width="18.38"/>
+    <col customWidth="1" min="6" max="6" width="20.38"/>
+    <col customWidth="1" min="7" max="7" width="17.0"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2667,635 +3030,723 @@
         <v>228</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E2" s="2">
-        <v>43832.125</v>
-      </c>
-      <c r="F2" s="3">
+      <c r="F2" s="2">
+        <v>43832.125</v>
+      </c>
+      <c r="G2" s="3">
         <v>43834.125</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="E3" s="2">
-        <v>43832.125</v>
-      </c>
-      <c r="F3" s="3">
+      <c r="F3" s="2">
+        <v>43832.125</v>
+      </c>
+      <c r="G3" s="3">
         <v>43835.125</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="E4" s="2">
-        <v>43832.125</v>
-      </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
+        <v>43832.125</v>
+      </c>
+      <c r="G4" s="3">
         <v>43875.125</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="E5" s="2">
-        <v>43832.125</v>
-      </c>
-      <c r="F5" s="3">
+      <c r="F5" s="2">
+        <v>43832.125</v>
+      </c>
+      <c r="G5" s="3">
         <v>43837.125</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="E6" s="2">
-        <v>43832.125</v>
-      </c>
-      <c r="F6" s="3">
+      <c r="F6" s="2">
+        <v>43832.125</v>
+      </c>
+      <c r="G6" s="3">
         <v>43875.125</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="E7" s="2">
+      <c r="F7" s="2">
         <v>43850.125</v>
       </c>
-      <c r="F7" s="3">
+      <c r="G7" s="3">
         <v>43895.125</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>241</v>
+        <v>248</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>242</v>
+        <v>249</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="E8" s="2">
+      <c r="F8" s="2">
         <v>43853.125</v>
       </c>
-      <c r="F8" s="3">
+      <c r="G8" s="3">
         <v>43859.125</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="4" t="s">
-        <v>243</v>
+        <v>251</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D9" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="E9" s="2">
+      <c r="F9" s="2">
         <v>43892.125</v>
       </c>
-      <c r="F9" s="3">
+      <c r="G9" s="3">
         <v>43924.125</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="s">
-        <v>245</v>
+        <v>254</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>246</v>
+        <v>255</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="E10" s="2">
+      <c r="F10" s="2">
         <v>43831.125</v>
       </c>
-      <c r="F10" s="3">
+      <c r="G10" s="3">
         <v>43834.125</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="4" t="s">
-        <v>247</v>
+        <v>257</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>248</v>
+        <v>258</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="E11" s="2">
+      <c r="F11" s="2">
         <v>44928.125</v>
       </c>
-      <c r="F11" s="3">
+      <c r="G11" s="3">
         <v>44932.125</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="s">
-        <v>249</v>
+        <v>260</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D12" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="E12" s="2">
+      <c r="F12" s="2">
         <v>45293.125</v>
       </c>
-      <c r="F12" s="3">
+      <c r="G12" s="3">
         <v>45349.125</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="4" t="s">
-        <v>251</v>
+        <v>263</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>252</v>
+        <v>264</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="E13" s="2">
+      <c r="F13" s="2">
         <v>44928.125</v>
       </c>
-      <c r="F13" s="3">
+      <c r="G13" s="3">
         <v>44973.125</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="4" t="s">
-        <v>253</v>
+        <v>266</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>254</v>
+        <v>267</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D14" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="E14" s="2">
+      <c r="F14" s="2">
         <v>43850.125</v>
       </c>
-      <c r="F14" s="3">
+      <c r="G14" s="3">
         <v>43904.125</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>255</v>
+        <v>269</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>256</v>
+        <v>270</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D15" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="E15" s="2">
+      <c r="F15" s="2">
         <v>43853.125</v>
       </c>
-      <c r="F15" s="3">
+      <c r="G15" s="3">
         <v>43856.125</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>257</v>
+        <v>272</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>258</v>
+        <v>273</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D16" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="E16" s="2">
-        <v>43832.125</v>
-      </c>
-      <c r="F16" s="3">
+      <c r="F16" s="2">
+        <v>43832.125</v>
+      </c>
+      <c r="G16" s="3">
         <v>43855.125</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>259</v>
+        <v>275</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>260</v>
+        <v>276</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D17" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="E17" s="2">
-        <v>43832.125</v>
-      </c>
-      <c r="F17" s="3">
+      <c r="F17" s="2">
+        <v>43832.125</v>
+      </c>
+      <c r="G17" s="3">
         <v>43886.125</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="4" t="s">
-        <v>261</v>
+        <v>278</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>262</v>
+        <v>279</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D18" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="E18" s="2">
-        <v>43832.125</v>
-      </c>
-      <c r="F18" s="3">
+      <c r="F18" s="2">
+        <v>43832.125</v>
+      </c>
+      <c r="G18" s="3">
         <v>43866.125</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>263</v>
+        <v>281</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>264</v>
+        <v>282</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D19" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="E19" s="2">
-        <v>43832.125</v>
-      </c>
-      <c r="F19" s="3">
+      <c r="F19" s="2">
+        <v>43832.125</v>
+      </c>
+      <c r="G19" s="3">
         <v>43888.125</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="4" t="s">
-        <v>265</v>
+        <v>284</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>266</v>
+        <v>285</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D20" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="E20" s="2">
+      <c r="F20" s="2">
         <v>43850.125</v>
       </c>
-      <c r="F20" s="3">
+      <c r="G20" s="3">
         <v>43852.125</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="4" t="s">
-        <v>267</v>
+      <c r="A21" s="1" t="s">
+        <v>287</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>268</v>
+        <v>288</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D21" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="E21" s="2">
+      <c r="F21" s="2">
         <v>43853.125</v>
       </c>
-      <c r="F21" s="3">
+      <c r="G21" s="3">
         <v>43887.125</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>269</v>
+        <v>290</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>270</v>
+        <v>291</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D22" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="E22" s="2">
+      <c r="F22" s="2">
         <v>43892.125</v>
       </c>
-      <c r="F22" s="3">
+      <c r="G22" s="3">
         <v>43946.125</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="4" t="s">
-        <v>271</v>
+      <c r="A23" s="1" t="s">
+        <v>293</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>272</v>
+        <v>294</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D23" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="E23" s="2">
+      <c r="F23" s="2">
         <v>43831.125</v>
       </c>
-      <c r="F23" s="3">
+      <c r="G23" s="3">
         <v>43852.125</v>
       </c>
     </row>
     <row r="24">
-      <c r="E24" s="2"/>
-      <c r="F24" s="3"/>
+      <c r="A24" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="F24" s="2">
+        <v>43853.125</v>
+      </c>
+      <c r="G24" s="2">
+        <v>43887.125</v>
+      </c>
     </row>
     <row r="25">
-      <c r="E25" s="2"/>
-      <c r="F25" s="3"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="3"/>
     </row>
     <row r="26">
-      <c r="E26" s="2"/>
-      <c r="F26" s="3"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="3"/>
     </row>
     <row r="27">
-      <c r="E27" s="2"/>
-      <c r="F27" s="3"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="3"/>
     </row>
     <row r="28">
-      <c r="E28" s="2"/>
-      <c r="F28" s="3"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="3"/>
     </row>
     <row r="29">
-      <c r="E29" s="2"/>
-      <c r="F29" s="3"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="3"/>
     </row>
     <row r="30">
-      <c r="E30" s="2"/>
-      <c r="F30" s="3"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="3"/>
     </row>
     <row r="31">
-      <c r="E31" s="2"/>
-      <c r="F31" s="3"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="3"/>
     </row>
     <row r="32">
-      <c r="E32" s="2"/>
-      <c r="F32" s="3"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="3"/>
     </row>
     <row r="33">
-      <c r="E33" s="2"/>
-      <c r="F33" s="3"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="3"/>
     </row>
     <row r="34">
-      <c r="E34" s="2"/>
-      <c r="F34" s="3"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="3"/>
     </row>
     <row r="35">
-      <c r="E35" s="2"/>
-      <c r="F35" s="3"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="3"/>
     </row>
     <row r="36">
-      <c r="E36" s="2"/>
-      <c r="F36" s="3"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="3"/>
     </row>
     <row r="37">
-      <c r="E37" s="2"/>
-      <c r="F37" s="3"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="3"/>
     </row>
     <row r="38">
-      <c r="E38" s="2"/>
-      <c r="F38" s="3"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="3"/>
     </row>
     <row r="39">
-      <c r="E39" s="2"/>
-      <c r="F39" s="3"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="3"/>
     </row>
     <row r="40">
-      <c r="E40" s="2"/>
-      <c r="F40" s="3"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="3"/>
     </row>
     <row r="41">
-      <c r="E41" s="2"/>
-      <c r="F41" s="3"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="3"/>
     </row>
     <row r="42">
-      <c r="E42" s="2"/>
-      <c r="F42" s="3"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="3"/>
     </row>
     <row r="43">
-      <c r="E43" s="2"/>
-      <c r="F43" s="3"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="3"/>
     </row>
     <row r="44">
-      <c r="E44" s="2"/>
-      <c r="F44" s="3"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="3"/>
     </row>
     <row r="45">
-      <c r="E45" s="2"/>
-      <c r="F45" s="3"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="3"/>
     </row>
     <row r="46">
-      <c r="E46" s="2"/>
-      <c r="F46" s="3"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="3"/>
     </row>
     <row r="47">
-      <c r="E47" s="2"/>
-      <c r="F47" s="3"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="3"/>
     </row>
     <row r="48">
-      <c r="E48" s="2"/>
-      <c r="F48" s="3"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="3"/>
     </row>
     <row r="49">
-      <c r="E49" s="2"/>
-      <c r="F49" s="3"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="3"/>
     </row>
     <row r="50">
-      <c r="E50" s="2"/>
-      <c r="F50" s="3"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="3"/>
     </row>
     <row r="51">
-      <c r="E51" s="2"/>
-      <c r="F51" s="3"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="3"/>
     </row>
     <row r="52">
-      <c r="E52" s="2"/>
-      <c r="F52" s="3"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="3"/>
     </row>
     <row r="53">
-      <c r="E53" s="2"/>
-      <c r="F53" s="3"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="3"/>
     </row>
     <row r="54">
-      <c r="E54" s="2"/>
-      <c r="F54" s="3"/>
+      <c r="F54" s="2"/>
+      <c r="G54" s="3"/>
     </row>
     <row r="55">
-      <c r="E55" s="2"/>
-      <c r="F55" s="3"/>
+      <c r="F55" s="2"/>
+      <c r="G55" s="3"/>
     </row>
     <row r="56">
-      <c r="E56" s="2"/>
-      <c r="F56" s="3"/>
+      <c r="F56" s="2"/>
+      <c r="G56" s="3"/>
     </row>
     <row r="57">
-      <c r="E57" s="2"/>
-      <c r="F57" s="3"/>
+      <c r="F57" s="2"/>
+      <c r="G57" s="3"/>
     </row>
     <row r="58">
-      <c r="E58" s="2"/>
-      <c r="F58" s="3"/>
+      <c r="F58" s="2"/>
+      <c r="G58" s="3"/>
     </row>
     <row r="59">
-      <c r="E59" s="2"/>
-      <c r="F59" s="3"/>
+      <c r="F59" s="2"/>
+      <c r="G59" s="3"/>
     </row>
     <row r="60">
-      <c r="E60" s="2"/>
-      <c r="F60" s="3"/>
+      <c r="F60" s="2"/>
+      <c r="G60" s="3"/>
     </row>
     <row r="61">
-      <c r="E61" s="2"/>
-      <c r="F61" s="3"/>
+      <c r="F61" s="2"/>
+      <c r="G61" s="3"/>
     </row>
     <row r="62">
-      <c r="E62" s="2"/>
-      <c r="F62" s="3"/>
+      <c r="F62" s="2"/>
+      <c r="G62" s="3"/>
     </row>
     <row r="63">
-      <c r="E63" s="2"/>
-      <c r="F63" s="3"/>
+      <c r="F63" s="2"/>
+      <c r="G63" s="3"/>
     </row>
     <row r="64">
-      <c r="E64" s="2"/>
-      <c r="F64" s="3"/>
+      <c r="F64" s="2"/>
+      <c r="G64" s="3"/>
     </row>
     <row r="65">
-      <c r="E65" s="2"/>
-      <c r="F65" s="3"/>
+      <c r="F65" s="2"/>
+      <c r="G65" s="3"/>
     </row>
     <row r="66">
-      <c r="E66" s="2"/>
-      <c r="F66" s="3"/>
+      <c r="F66" s="2"/>
+      <c r="G66" s="3"/>
     </row>
     <row r="67">
-      <c r="E67" s="2"/>
-      <c r="F67" s="3"/>
+      <c r="F67" s="2"/>
+      <c r="G67" s="3"/>
     </row>
     <row r="68">
-      <c r="E68" s="2"/>
-      <c r="F68" s="3"/>
+      <c r="F68" s="2"/>
+      <c r="G68" s="3"/>
     </row>
     <row r="69">
-      <c r="E69" s="2"/>
-      <c r="F69" s="3"/>
+      <c r="F69" s="2"/>
+      <c r="G69" s="3"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -3322,13 +3773,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>273</v>
+        <v>298</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>274</v>
+        <v>299</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>275</v>
+        <v>300</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -3339,10 +3790,10 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>276</v>
+        <v>301</v>
       </c>
       <c r="C2" s="1">
         <v>4.0</v>
@@ -3359,10 +3810,10 @@
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>277</v>
+        <v>302</v>
       </c>
       <c r="C3" s="1">
         <v>5.0</v>
@@ -3379,10 +3830,10 @@
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>278</v>
+        <v>303</v>
       </c>
       <c r="C4" s="1">
         <v>3.0</v>
@@ -3399,10 +3850,10 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>279</v>
+        <v>304</v>
       </c>
       <c r="C5" s="1">
         <v>4.0</v>
@@ -3419,10 +3870,10 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>280</v>
+        <v>305</v>
       </c>
       <c r="C6" s="1">
         <v>5.0</v>
@@ -3439,10 +3890,10 @@
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>281</v>
+        <v>306</v>
       </c>
       <c r="C7" s="1">
         <v>5.0</v>
@@ -3459,10 +3910,10 @@
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>241</v>
+        <v>248</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>282</v>
+        <v>307</v>
       </c>
       <c r="C8" s="1">
         <v>4.0</v>
@@ -3479,10 +3930,10 @@
     </row>
     <row r="9">
       <c r="A9" s="4" t="s">
-        <v>243</v>
+        <v>251</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>283</v>
+        <v>308</v>
       </c>
       <c r="C9" s="1">
         <v>3.0</v>
@@ -3499,10 +3950,10 @@
     </row>
     <row r="10">
       <c r="A10" s="4" t="s">
-        <v>245</v>
+        <v>254</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>284</v>
+        <v>309</v>
       </c>
       <c r="C10" s="1">
         <v>4.0</v>
@@ -3519,10 +3970,10 @@
     </row>
     <row r="11">
       <c r="A11" s="4" t="s">
-        <v>247</v>
+        <v>257</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>285</v>
+        <v>310</v>
       </c>
       <c r="C11" s="1">
         <v>4.0</v>
@@ -3539,10 +3990,10 @@
     </row>
     <row r="12">
       <c r="A12" s="4" t="s">
-        <v>249</v>
+        <v>260</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>286</v>
+        <v>311</v>
       </c>
       <c r="C12" s="1">
         <v>4.0</v>
@@ -3559,10 +4010,10 @@
     </row>
     <row r="13">
       <c r="A13" s="4" t="s">
-        <v>251</v>
+        <v>263</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>287</v>
+        <v>312</v>
       </c>
       <c r="C13" s="1">
         <v>5.0</v>
@@ -3579,10 +4030,10 @@
     </row>
     <row r="14">
       <c r="A14" s="4" t="s">
-        <v>253</v>
+        <v>266</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>288</v>
+        <v>313</v>
       </c>
       <c r="C14" s="1">
         <v>5.0</v>
@@ -3599,10 +4050,10 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>255</v>
+        <v>314</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>289</v>
+        <v>315</v>
       </c>
       <c r="C15" s="1">
         <v>4.0</v>
@@ -3619,10 +4070,10 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>257</v>
+        <v>272</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>290</v>
+        <v>316</v>
       </c>
       <c r="C16" s="1">
         <v>4.0</v>
@@ -3639,10 +4090,10 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>259</v>
+        <v>275</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>291</v>
+        <v>317</v>
       </c>
       <c r="C17" s="1">
         <v>5.0</v>
@@ -3659,10 +4110,10 @@
     </row>
     <row r="18">
       <c r="A18" s="4" t="s">
-        <v>261</v>
+        <v>278</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>292</v>
+        <v>318</v>
       </c>
       <c r="C18" s="1">
         <v>3.0</v>
@@ -3679,10 +4130,10 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>263</v>
+        <v>281</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>293</v>
+        <v>319</v>
       </c>
       <c r="C19" s="1">
         <v>4.0</v>
@@ -3699,10 +4150,10 @@
     </row>
     <row r="20">
       <c r="A20" s="4" t="s">
-        <v>265</v>
+        <v>284</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>294</v>
+        <v>320</v>
       </c>
       <c r="C20" s="1">
         <v>4.0</v>
@@ -3719,10 +4170,10 @@
     </row>
     <row r="21">
       <c r="A21" s="4" t="s">
-        <v>267</v>
+        <v>321</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>295</v>
+        <v>322</v>
       </c>
       <c r="C21" s="1">
         <v>4.0</v>
@@ -3739,10 +4190,10 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>269</v>
+        <v>290</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>296</v>
+        <v>323</v>
       </c>
       <c r="C22" s="1">
         <v>5.0</v>
@@ -3759,10 +4210,10 @@
     </row>
     <row r="23">
       <c r="A23" s="4" t="s">
-        <v>271</v>
+        <v>324</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>297</v>
+        <v>325</v>
       </c>
       <c r="C23" s="1">
         <v>5.0</v>
@@ -3779,10 +4230,10 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>298</v>
+        <v>326</v>
       </c>
       <c r="C24" s="1">
         <v>5.0</v>
@@ -3799,10 +4250,10 @@
     </row>
     <row r="25">
       <c r="A25" s="4" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>299</v>
+        <v>327</v>
       </c>
       <c r="C25" s="1">
         <v>5.0</v>
@@ -3819,10 +4270,10 @@
     </row>
     <row r="26">
       <c r="A26" s="4" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>300</v>
+        <v>328</v>
       </c>
       <c r="C26" s="1">
         <v>4.0</v>
@@ -3839,10 +4290,10 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>301</v>
+        <v>329</v>
       </c>
       <c r="C27" s="1">
         <v>5.0</v>
@@ -3859,10 +4310,10 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>302</v>
+        <v>330</v>
       </c>
       <c r="C28" s="1">
         <v>5.0</v>
@@ -3879,10 +4330,10 @@
     </row>
     <row r="29">
       <c r="A29" s="4" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>303</v>
+        <v>331</v>
       </c>
       <c r="C29" s="1">
         <v>5.0</v>
@@ -3899,10 +4350,10 @@
     </row>
     <row r="30">
       <c r="A30" s="4" t="s">
-        <v>241</v>
+        <v>248</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>304</v>
+        <v>332</v>
       </c>
       <c r="C30" s="1">
         <v>4.0</v>
@@ -3919,10 +4370,10 @@
     </row>
     <row r="31">
       <c r="A31" s="4" t="s">
-        <v>243</v>
+        <v>251</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>305</v>
+        <v>333</v>
       </c>
       <c r="C31" s="1">
         <v>3.0</v>
@@ -3939,10 +4390,10 @@
     </row>
     <row r="32">
       <c r="A32" s="4" t="s">
-        <v>245</v>
+        <v>254</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>306</v>
+        <v>334</v>
       </c>
       <c r="C32" s="1">
         <v>4.0</v>
@@ -3959,10 +4410,10 @@
     </row>
     <row r="33">
       <c r="A33" s="4" t="s">
-        <v>247</v>
+        <v>257</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>307</v>
+        <v>335</v>
       </c>
       <c r="C33" s="1">
         <v>4.0</v>
@@ -3979,10 +4430,10 @@
     </row>
     <row r="34">
       <c r="A34" s="4" t="s">
-        <v>249</v>
+        <v>260</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>308</v>
+        <v>336</v>
       </c>
       <c r="C34" s="1">
         <v>5.0</v>
@@ -3999,10 +4450,10 @@
     </row>
     <row r="35">
       <c r="A35" s="4" t="s">
-        <v>251</v>
+        <v>263</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>309</v>
+        <v>337</v>
       </c>
       <c r="C35" s="1">
         <v>5.0</v>
@@ -4019,10 +4470,10 @@
     </row>
     <row r="36">
       <c r="A36" s="4" t="s">
-        <v>253</v>
+        <v>266</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>310</v>
+        <v>338</v>
       </c>
       <c r="C36" s="1">
         <v>4.0</v>
@@ -4039,10 +4490,10 @@
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>255</v>
+        <v>314</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>311</v>
+        <v>339</v>
       </c>
       <c r="C37" s="1">
         <v>5.0</v>
@@ -4059,10 +4510,10 @@
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>257</v>
+        <v>272</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>312</v>
+        <v>340</v>
       </c>
       <c r="C38" s="1">
         <v>4.0</v>
@@ -4079,10 +4530,10 @@
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>259</v>
+        <v>275</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>313</v>
+        <v>341</v>
       </c>
       <c r="C39" s="1">
         <v>4.0</v>
@@ -4099,10 +4550,10 @@
     </row>
     <row r="40">
       <c r="A40" s="4" t="s">
-        <v>261</v>
+        <v>278</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>314</v>
+        <v>342</v>
       </c>
       <c r="C40" s="1">
         <v>5.0</v>
@@ -4119,10 +4570,10 @@
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>263</v>
+        <v>281</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>315</v>
+        <v>343</v>
       </c>
       <c r="C41" s="1">
         <v>4.0</v>
@@ -4139,10 +4590,10 @@
     </row>
     <row r="42">
       <c r="A42" s="4" t="s">
-        <v>265</v>
+        <v>284</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>316</v>
+        <v>344</v>
       </c>
       <c r="C42" s="1">
         <v>5.0</v>
@@ -4159,10 +4610,10 @@
     </row>
     <row r="43">
       <c r="A43" s="4" t="s">
-        <v>267</v>
+        <v>321</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>317</v>
+        <v>345</v>
       </c>
       <c r="C43" s="1">
         <v>3.0</v>
@@ -4179,10 +4630,10 @@
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>269</v>
+        <v>290</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>318</v>
+        <v>346</v>
       </c>
       <c r="C44" s="1">
         <v>4.0</v>
@@ -4199,10 +4650,10 @@
     </row>
     <row r="45">
       <c r="A45" s="4" t="s">
-        <v>271</v>
+        <v>324</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>319</v>
+        <v>347</v>
       </c>
       <c r="C45" s="1">
         <v>5.0</v>
@@ -4338,7 +4789,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>320</v>
+        <v>348</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -4352,13 +4803,13 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>321</v>
+        <v>349</v>
       </c>
       <c r="B2" s="1">
         <v>4.0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>322</v>
+        <v>350</v>
       </c>
       <c r="D2" s="2">
         <v>43832.125</v>
@@ -4369,13 +4820,13 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>323</v>
+        <v>351</v>
       </c>
       <c r="B3" s="1">
         <v>3.0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>324</v>
+        <v>352</v>
       </c>
       <c r="D3" s="2">
         <v>43832.125</v>
@@ -4386,13 +4837,13 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>325</v>
+        <v>353</v>
       </c>
       <c r="B4" s="1">
         <v>2.0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>326</v>
+        <v>354</v>
       </c>
       <c r="D4" s="2">
         <v>43832.125</v>
@@ -4403,13 +4854,13 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>327</v>
+        <v>355</v>
       </c>
       <c r="B5" s="1">
         <v>1.0</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>328</v>
+        <v>356</v>
       </c>
       <c r="D5" s="2">
         <v>43832.125</v>

</xml_diff>

<commit_message>
fix: add missing column id_establishemnt to ratings and edit comment to review as entity reviews. Teste are passed
</commit_message>
<xml_diff>
--- a/seeds/seeds.xlsx
+++ b/seeds/seeds.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="426">
   <si>
     <t>id</t>
   </si>
@@ -701,6 +701,9 @@
     <t>id_type</t>
   </si>
   <si>
+    <t>description</t>
+  </si>
+  <si>
     <t>address</t>
   </si>
   <si>
@@ -713,6 +716,9 @@
     <t>Cinelândia</t>
   </si>
   <si>
+    <t>O melhor ponto de encontro cultural no coração do Rio de Janeiro. Venha desfrutar de filmes, teatro e música em um ambiente acolhedor e sofisticado. Imperdível!</t>
+  </si>
+  <si>
     <t>Rua Dos Filmes, 324</t>
   </si>
   <si>
@@ -722,6 +728,9 @@
     <t>Restaurante da Rose</t>
   </si>
   <si>
+    <t>O Restaurante da Rose é o lugar perfeito para saborear pratos deliciosos e autênticos. Com um ambiente acolhedor e atendimento impecável, garantimos uma experiência gastronômica única. Venha nos visitar e desfrute de momentos inesquecíveis!</t>
+  </si>
+  <si>
     <t>Avenida dos Pratos, 123</t>
   </si>
   <si>
@@ -731,6 +740,9 @@
     <t>Parquemania</t>
   </si>
   <si>
+    <t>Parquemania - O melhor parque de diversões da cidade! Venha se divertir em nossos brinquedos radicais e aproveite nossas deliciosas opções gastronômicas. Uma experiência inesquecível para toda a família!</t>
+  </si>
+  <si>
     <t>Rua da Alegria, 123</t>
   </si>
   <si>
@@ -740,6 +752,9 @@
     <t>Parque da Criança</t>
   </si>
   <si>
+    <t>O Parque da Criança é o lugar perfeito para a diversão em família! Com diversas opções de brinquedos e atividades, as crianças vão se divertir muito enquanto os pais relaxam em um ambiente seguro e agradável. Venha nos visitar e aproveite o melhor do lazer em família! #ParqueDaCriança #DiversãoEmFamília #LazerSeguro</t>
+  </si>
+  <si>
     <t>Rua Central, 32</t>
   </si>
   <si>
@@ -749,6 +764,9 @@
     <t>Museu do espaço</t>
   </si>
   <si>
+    <t>O Museu do Espaço é o lugar perfeito para explorar o universo! Com exposições interativas e incríveis réplicas de naves espaciais, proporcionamos uma experiência única para os amantes da astronomia. Venha nos visitar e embarque nessa jornada fascinante pelo cosmos!</t>
+  </si>
+  <si>
     <t>Avenida da descoberta, 123</t>
   </si>
   <si>
@@ -758,6 +776,9 @@
     <t>Teatro Rural</t>
   </si>
   <si>
+    <t>O Teatro Rural é um espaço encantador que oferece espetáculos emocionantes e divertidos para toda a família. Venha se encantar com nossas peças teatrais e desfrute de momentos inesquecíveis em meio à natureza. Aproveite também nossa deliciosa gastronomia e ambiente acolhedor. Esperamos por você!</t>
+  </si>
+  <si>
     <t>Rua dos Bois, 23</t>
   </si>
   <si>
@@ -767,6 +788,9 @@
     <t>Zoo Safari a Dentro</t>
   </si>
   <si>
+    <t>O Zoo Safari a Dentro é o lugar perfeito para se conectar com a natureza e os animais. Desfrute de uma experiência única e emocionante, onde você pode observar de perto diversas espécies em seu habitat natural. Venha nos visitar e viva momentos inesquecíveis!</t>
+  </si>
+  <si>
     <t>Avenida da Selva, 32</t>
   </si>
   <si>
@@ -776,6 +800,9 @@
     <t>Lagoa Azul</t>
   </si>
   <si>
+    <t>O paraíso na terra! A Lagoa Azul é o refúgio perfeito para relaxar e se reconectar com a natureza. Desfrute de águas cristalinas, areia branca e uma paisagem deslumbrante. Venha viver momentos inesquecíveis em nosso paraíso tropical!</t>
+  </si>
+  <si>
     <t>Rua da Criança, 43</t>
   </si>
   <si>
@@ -785,6 +812,9 @@
     <t>Serra dos Cavalos</t>
   </si>
   <si>
+    <t>Venha conhecer a Serra dos Cavalos, o refúgio perfeito para os amantes da natureza. Desfrute de trilhas deslumbrantes, cachoeiras encantadoras e uma vista panorâmica de tirar o fôlego. Aventure-se nesse paraíso e viva momentos inesquecíveis. #SerraDosCavalos #Natureza</t>
+  </si>
+  <si>
     <t>Trila ecológica do cavalo</t>
   </si>
   <si>
@@ -794,6 +824,9 @@
     <t>Veneza Parque</t>
   </si>
   <si>
+    <t>O Veneza Parque é o lugar perfeito para se divertir em família. Com uma ampla variedade de atrações, como piscinas, toboáguas e áreas de lazer, garantimos momentos inesquecíveis. Venha nos visitar e aproveite o melhor do entretenimento!</t>
+  </si>
+  <si>
     <t>Rodovia das Águas, km 34</t>
   </si>
   <si>
@@ -803,6 +836,9 @@
     <t>Centro de descobertas</t>
   </si>
   <si>
+    <t>O Centro de Descobertas é o lugar perfeito para explorar e aprender. Com uma variedade de atividades interativas e educativas, oferecemos uma experiência única para todas as idades. Venha descobrir conosco!</t>
+  </si>
+  <si>
     <t>Rua da descoberta, 32</t>
   </si>
   <si>
@@ -812,6 +848,9 @@
     <t>Museu das Artes</t>
   </si>
   <si>
+    <t>O Museu das Artes é um lugar encantador que abriga uma vasta coleção de obras de arte. Venha explorar a história e a cultura através de exposições fascinantes. Desfrute de um ambiente acolhedor e descubra a beleza da arte em cada detalhe. Visite-nos e deixe-se inspirar!</t>
+  </si>
+  <si>
     <t>Rua do Cateiro, 211</t>
   </si>
   <si>
@@ -821,6 +860,9 @@
     <t>Jardim Botanico da Cidade</t>
   </si>
   <si>
+    <t>"O Jardim Botânico da Cidade é um refúgio encantador para os amantes da natureza. Com uma variedade deslumbrante de plantas e flores, este paraíso verde oferece tranquilidade e beleza em cada passo. Venha explorar e se maravilhar com a exuberância deste lugar único!" (300 caracteres)</t>
+  </si>
+  <si>
     <t>Rodovia Luiz Gonzaga, 43</t>
   </si>
   <si>
@@ -830,6 +872,9 @@
     <t xml:space="preserve">Patinaço </t>
   </si>
   <si>
+    <t>O melhor lugar para patinar em São Paulo! Venha se divertir e praticar suas habilidades no gelo conosco. Ambiente familiar e seguro para todas as idades. Não perca a oportunidade de conhecer o Patinaço!</t>
+  </si>
+  <si>
     <t>Shopping da Cidade, 12</t>
   </si>
   <si>
@@ -839,6 +884,9 @@
     <t xml:space="preserve">Fliperama </t>
   </si>
   <si>
+    <t>"O Fliperama é o lugar perfeito para se divertir com amigos e família! Com nossas máquinas de jogos clássicos e modernos, você pode passar horas se divertindo. Além disso, oferecemos deliciosos lanches e bebidas para acompanhar sua diversão. Venha nos visitar e experimente a emoção do Fliperama!" (caracteres: 296)</t>
+  </si>
+  <si>
     <t>Avenida dos Jogos, 34</t>
   </si>
   <si>
@@ -848,6 +896,9 @@
     <t>Museu da Criaça</t>
   </si>
   <si>
+    <t>O Museu da Criança é o lugar perfeito para a diversão em família! Com diversas atividades interativas, as crianças podem aprender enquanto se divertem. Venha conhecer nossas exposições e se encantar com o mundo da imaginação. #MuseudaCriança #DiversãoemFamília #ExperiênciaInterativa</t>
+  </si>
+  <si>
     <t>Rua da história, 11</t>
   </si>
   <si>
@@ -857,6 +908,9 @@
     <t>Picinic da Sol</t>
   </si>
   <si>
+    <t>O Picnic da Sol é o lugar perfeito para desfrutar de momentos ao ar livre. Com uma atmosfera acolhedora e uma variedade de opções de alimentos frescos e deliciosos, você vai se sentir em um verdadeiro paraíso gastronômico. Venha aproveitar o sol e saborear nossas delícias!</t>
+  </si>
+  <si>
     <t>Praça da Iluminação, centro</t>
   </si>
   <si>
@@ -866,6 +920,9 @@
     <t>Baobá</t>
   </si>
   <si>
+    <t>O Baobá é o lugar perfeito para relaxar e desfrutar de deliciosos coquetéis e petiscos. Venha nos visitar e aproveite nossa atmosfera acolhedora e música ao vivo todas as sextas-feiras!</t>
+  </si>
+  <si>
     <t>Rua da  Selva, 42</t>
   </si>
   <si>
@@ -875,6 +932,9 @@
     <t>Rancho Alegre</t>
   </si>
   <si>
+    <t>O Rancho Alegre é o lugar perfeito para desfrutar de deliciosas refeições caseiras. Com um ambiente acolhedor e atendimento impecável, oferecemos pratos tradicionais da culinária brasileira. Venha nos visitar e saborear o melhor da gastronomia em um ambiente familiar e aconchegante.</t>
+  </si>
+  <si>
     <t>Avenida do Rancho, 235</t>
   </si>
   <si>
@@ -884,6 +944,9 @@
     <t>Piscinão Azul</t>
   </si>
   <si>
+    <t>O Piscinão Azul é o lugar perfeito para relaxar e se refrescar. Com uma piscina cristalina e um ambiente acolhedor, oferecemos o melhor em entretenimento aquático. Venha nos visitar e desfrute de momentos inesquecíveis!</t>
+  </si>
+  <si>
     <t>Rua dos clubes, 32</t>
   </si>
   <si>
@@ -893,6 +956,9 @@
     <t>Burguelândia</t>
   </si>
   <si>
+    <t>Venha experimentar os melhores hambúrgueres artesanais da cidade! Com ingredientes frescos e um ambiente descontraído, Burguelândia é o lugar perfeito para satisfazer seu desejo por um delicioso lanche. Não perca tempo, faça uma visita e descubra o sabor que vai te conquistar!</t>
+  </si>
+  <si>
     <t>Rua das comidas, 43</t>
   </si>
   <si>
@@ -902,15 +968,24 @@
     <t>Pizzamania</t>
   </si>
   <si>
+    <t>Venha experimentar as melhores pizzas da cidade! Com uma variedade de sabores irresistíveis e ingredientes frescos, a Pizzamania é o lugar perfeito para satisfazer seu desejo por pizza. Ambiente acolhedor e atendimento de primeira. Não perca tempo, faça sua reserva agora mesmo!</t>
+  </si>
+  <si>
     <t>uuid-casa-club</t>
   </si>
   <si>
     <t>Casa Club</t>
   </si>
   <si>
+    <t>A Casa Club é o lugar perfeito para quem busca diversão e entretenimento. Com uma decoração moderna e sofisticada, oferecemos uma ampla variedade de bebidas e petiscos deliciosos. Venha curtir a noite conosco e aproveite nossas promoções especiais!</t>
+  </si>
+  <si>
     <t>Rua dos clubes, 45</t>
   </si>
   <si>
+    <t>id_establishment</t>
+  </si>
+  <si>
     <t>review</t>
   </si>
   <si>
@@ -920,142 +995,274 @@
     <t>id_user</t>
   </si>
   <si>
+    <t>uuid-review-1</t>
+  </si>
+  <si>
     <t>Um lugar incrível para os amantes de cinema! A qualidade do som e da imagem é excelente, e a seleção de filmes sempre inclui os últimos lançamentos.</t>
   </si>
   <si>
+    <t>uuid-review-2</t>
+  </si>
+  <si>
     <t>Comida caseira autêntica e um ambiente acolhedor. A Rose faz você se sentir em casa. Não deixe de provar o estrogonofe!</t>
   </si>
   <si>
+    <t>uuid-review-3</t>
+  </si>
+  <si>
     <t>Um parque de diversões que superou todas as nossas expectativas! Ideal para todas as idades, com muitas atrações radicais e áreas temáticas.</t>
   </si>
   <si>
+    <t>uuid-review-4</t>
+  </si>
+  <si>
     <t>Perfeito para um dia em família! Muitas atividades interativas para as crianças e espaços de descanso para os adultos</t>
   </si>
   <si>
+    <t>uuid-review-5</t>
+  </si>
+  <si>
     <t>Fascinante! A exposição interativa é uma jornada incrível pelo universo. Recomendo muito para quem tem interesse em astronomia</t>
   </si>
   <si>
+    <t>uuid-review-6</t>
+  </si>
+  <si>
     <t>Uma experiência única que combina arte e natureza. As peças são sempre emocionantes e o cenário ao ar livre é deslumbrante.</t>
   </si>
   <si>
+    <t>uuid-review-7</t>
+  </si>
+  <si>
     <t>Uma experiência inesquecível! Ver os animais tão de perto foi emocionante. Excelente programa para as crianças aprenderem sobre conservação.</t>
   </si>
   <si>
+    <t>uuid-review-8</t>
+  </si>
+  <si>
     <t>Um oásis de tranquilidade. Águas cristalinas e perfeitas para um mergulho refrescante. Um lugar maravilhoso para relaxar e se conectar com a natureza.</t>
   </si>
   <si>
+    <t>uuid-review-9</t>
+  </si>
+  <si>
     <t>Para os aventureiros de plantão, a Serra dos Cavalos oferece trilhas desafiadoras com vistas de tirar o fôlego. Vale cada passo!</t>
   </si>
   <si>
+    <t>uuid-review-10</t>
+  </si>
+  <si>
     <t>Uma mini-Veneza que encanta a todos. Os passeios de gôndola são românticos e a arquitetura é impressionante. Um pedacinho da Itália na cidade</t>
   </si>
   <si>
+    <t>uuid-review-11</t>
+  </si>
+  <si>
     <t>Interativo e educativo, é o lugar ideal para crianças curiosas. As exposições mudam frequentemente, sempre trazendo novidades</t>
   </si>
   <si>
+    <t>uuid-review-12</t>
+  </si>
+  <si>
     <t>Um espaço sublime que abriga coleções de arte impressionantes. A cada visita, descubro algo novo. Uma jóia cultural.</t>
   </si>
   <si>
+    <t>uuid-review-13</t>
+  </si>
+  <si>
     <t>Um refúgio verde no meio da cidade. A diversidade de plantas e flores é estonteante, e os caminhos são perfeitos para uma caminhada tranquila.</t>
   </si>
   <si>
+    <t>uuid-review-14</t>
+  </si>
+  <si>
     <t>uuid-patinaço</t>
   </si>
   <si>
     <t>A pista de patinação é ampla e bem cuidada. Um lugar divertido para famílias e amigos. Eles também oferecem aulas para iniciantes</t>
   </si>
   <si>
+    <t>uuid-review-15</t>
+  </si>
+  <si>
     <t>Voltar no tempo e reviver a infância. O fliperama tem uma ótima seleção de jogos clássicos e novos. Ótimo lugar para se divertir.</t>
   </si>
   <si>
+    <t>uuid-review-16</t>
+  </si>
+  <si>
     <t>Um lugar mágico cheio de atividades lúdicas e educativas. Meus filhos amaram e aprenderam muito brincando.</t>
   </si>
   <si>
+    <t>uuid-review-17</t>
+  </si>
+  <si>
     <t>O local perfeito para um piquenique em família ou com amigos. Muita grama verde, sombras agradáveis e uma vista deslumbrante do pôr do sol.</t>
   </si>
   <si>
+    <t>uuid-review-18</t>
+  </si>
+  <si>
     <t>Visitar o Baobá é como entrar em um conto de fadas. A árvore é majestosa e o ambiente ao redor é pacífico. Uma experiência memorável.</t>
   </si>
   <si>
+    <t>uuid-review-19</t>
+  </si>
+  <si>
     <t>Um dia no campo cheio de diversão e aprendizado. As atividades de fazenda são ótimas para as crianças, e os funcionários são super simpáticos.</t>
   </si>
   <si>
+    <t>uuid-review-20</t>
+  </si>
+  <si>
     <t>uuid-piscinão-azul</t>
   </si>
   <si>
     <t>A melhor fuga do calor! O parque aquático tem opções para todos, desde piscinas tranquilas até escorregadores emocionantes.</t>
   </si>
   <si>
+    <t>uuid-review-21</t>
+  </si>
+  <si>
     <t>O paraíso dos hambúrgueres! Cada opção no menu é mais deliciosa que a outra. O ambiente é descontraído e perfeito para encontros</t>
   </si>
   <si>
+    <t>uuid-review-22</t>
+  </si>
+  <si>
     <t>uuid-pizzarolla</t>
   </si>
   <si>
     <t>Uma pizzaria que se destaca. A massa fina e crocante e os ingredientes frescos fazem toda a diferença. Excelente atendimento também</t>
   </si>
   <si>
+    <t>uuid-review-23</t>
+  </si>
+  <si>
     <t>Ambiente confortável e aconchegante, com uma grande variedade de filmes. Os assentos são extremamente confortáveis e o atendimento é top.</t>
   </si>
   <si>
+    <t>uuid-review-24</t>
+  </si>
+  <si>
     <t>A sensação de comer na casa de uma amiga. O ambiente é simples, mas a comida é de primeira. O bolo de chocolate é imperdível!</t>
   </si>
   <si>
+    <t>uuid-review-25</t>
+  </si>
+  <si>
     <t>Um dia cheio de risadas e diversão garantida para toda a família. As atrações são seguras e bem mantidas, e o staff é super atencioso.</t>
   </si>
   <si>
+    <t>uuid-review-26</t>
+  </si>
+  <si>
     <t>Adorável! Muito limpo e seguro, com inúmeras atividades para manter as crianças entretidas. Os brinquedos educativos são um bônus.</t>
   </si>
   <si>
+    <t>uuid-review-27</t>
+  </si>
+  <si>
     <t>O show do planetário é simplesmente hipnotizante. Uma ótima maneira de passar a tarde aprendendo sobre as maravilhas do universo.</t>
   </si>
   <si>
+    <t>uuid-review-28</t>
+  </si>
+  <si>
     <t>Uma joia escondida. Assistir a uma peça aqui é uma experiência íntima e especial, com o cenário natural acrescentando ao espetáculo.</t>
   </si>
   <si>
+    <t>uuid-review-29</t>
+  </si>
+  <si>
     <t>Além de ver os animais, as crianças podem participar de atividades educativas. Os guias são apaixonados e muito informados.</t>
   </si>
   <si>
+    <t>uuid-review-30</t>
+  </si>
+  <si>
     <t>Um pedacinho do paraíso. Perfeito para nadar, fazer piquenique e simplesmente relaxar ao sol. As águas são surpreendentemente claras.</t>
   </si>
   <si>
+    <t>uuid-review-31</t>
+  </si>
+  <si>
     <t>As vistas do topo são de tirar o fôlego. Vale a pena o esforço da caminhada. Um ótimo lugar para desconnectar da rotina agitada.</t>
   </si>
   <si>
+    <t>uuid-review-32</t>
+  </si>
+  <si>
     <t>O detalhe e o cuidado na construção deste parque são incríveis. Sentimos como se estivéssemos realmente em Veneza por algumas horas.</t>
   </si>
   <si>
+    <t>uuid-review-33</t>
+  </si>
+  <si>
     <t>Cada visita é uma nova aventura. As crianças adoram os workshops práticos. É maravilhoso ver a curiosidade delas sendo estimulada.</t>
   </si>
   <si>
+    <t>uuid-review-34</t>
+  </si>
+  <si>
     <t>Perfeito para os amantes de arte. O museu oferece uma vasta coleção que abrange várias eras e estilos. Inspirador e educativo.</t>
   </si>
   <si>
+    <t>uuid-review-35</t>
+  </si>
+  <si>
     <t>Excelente lugar para uma caminhada tranquila ou uma corrida matinal. A diversidade de plantas e o layout são simplesmente impressionantes.</t>
   </si>
   <si>
+    <t>uuid-review-36</t>
+  </si>
+  <si>
     <t>Ambiente divertido e acolhedor, ideal para patinadores de todos os níveis. Eles também fazem festas de aniversário incríveis aqui.</t>
   </si>
   <si>
+    <t>uuid-review-37</t>
+  </si>
+  <si>
     <t>Um excelente lugar para reunir os amigos e desfrutar de uma competição amigável. Os jogos retro são os meus favoritos.</t>
   </si>
   <si>
+    <t>uuid-review-38</t>
+  </si>
+  <si>
     <t>Este lugar é um tesouro. As exposições interativas mantêm as crianças engajadas e aprendendo. A área de brincar ao ar livre é fantástica.</t>
   </si>
   <si>
+    <t>uuid-review-39</t>
+  </si>
+  <si>
     <t>O cenário é pitoresco, ideal para uma tarde relaxante. É um dos nossos locais favoritos para escapar da correria da cidade.</t>
   </si>
   <si>
+    <t>uuid-review-40</t>
+  </si>
+  <si>
     <t>Este lugar tem uma energia especial. A grandiosidade do Baobá te faz sentir pequeno e admirado. Ótimo para fotos e momentos de reflexão.</t>
   </si>
   <si>
+    <t>uuid-review-41</t>
+  </si>
+  <si>
     <t>A interação com os animais foi maravilhosa, especialmente para as crianças. Uma ótima maneira de aprender sobre a vida no campo.</t>
   </si>
   <si>
+    <t>uuid-review-42</t>
+  </si>
+  <si>
     <t>Limpo, divertido e refrescante. A variedade de piscinas atende a todos, e os tobogãs são emocionantes. Uma ótima maneira de passar o dia.</t>
   </si>
   <si>
+    <t>uuid-review-43</t>
+  </si>
+  <si>
     <t>As opções de hambúrgueres são criativas e deliciosas. O ambiente é vibrante e convidativo, perfeito para uma noite casual com amigos.</t>
+  </si>
+  <si>
+    <t>uuid-review-44</t>
   </si>
   <si>
     <t>Ambiente acolhedor com pizzas excepcionais. A seleção de coberturas é vasta e saborosa. Definitivamente, um dos melhores lugares da cidade.</t>
@@ -3010,10 +3217,11 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="23.38"/>
     <col customWidth="1" min="2" max="2" width="20.5"/>
-    <col customWidth="1" min="3" max="3" width="27.0"/>
-    <col customWidth="1" min="4" max="5" width="18.38"/>
-    <col customWidth="1" min="6" max="6" width="20.38"/>
-    <col customWidth="1" min="7" max="7" width="17.0"/>
+    <col customWidth="1" min="3" max="3" width="14.5"/>
+    <col customWidth="1" min="4" max="4" width="563.75"/>
+    <col customWidth="1" min="5" max="6" width="18.38"/>
+    <col customWidth="1" min="7" max="7" width="20.38"/>
+    <col customWidth="1" min="8" max="8" width="17.0"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3033,720 +3241,792 @@
         <v>229</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>232</v>
+      <c r="D2" s="4" t="s">
+        <v>233</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="F2" s="2">
-        <v>43832.125</v>
-      </c>
-      <c r="G2" s="3">
+      <c r="G2" s="2">
+        <v>43832.125</v>
+      </c>
+      <c r="H2" s="3">
         <v>43834.125</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>235</v>
+      <c r="D3" s="4" t="s">
+        <v>237</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="F3" s="2">
-        <v>43832.125</v>
-      </c>
-      <c r="G3" s="3">
+      <c r="G3" s="2">
+        <v>43832.125</v>
+      </c>
+      <c r="H3" s="3">
         <v>43835.125</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>238</v>
+      <c r="D4" s="4" t="s">
+        <v>241</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="F4" s="2">
-        <v>43832.125</v>
-      </c>
-      <c r="G4" s="3">
+      <c r="G4" s="2">
+        <v>43832.125</v>
+      </c>
+      <c r="H4" s="3">
         <v>43875.125</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>241</v>
+      <c r="D5" s="4" t="s">
+        <v>245</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="F5" s="2">
-        <v>43832.125</v>
-      </c>
-      <c r="G5" s="3">
+      <c r="G5" s="2">
+        <v>43832.125</v>
+      </c>
+      <c r="H5" s="3">
         <v>43837.125</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>244</v>
+      <c r="D6" s="4" t="s">
+        <v>249</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="F6" s="2">
-        <v>43832.125</v>
-      </c>
-      <c r="G6" s="3">
+      <c r="G6" s="2">
+        <v>43832.125</v>
+      </c>
+      <c r="H6" s="3">
         <v>43875.125</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>247</v>
+      <c r="D7" s="4" t="s">
+        <v>253</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="F7" s="2">
+      <c r="G7" s="2">
         <v>43850.125</v>
       </c>
-      <c r="G7" s="3">
+      <c r="H7" s="3">
         <v>43895.125</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>248</v>
+        <v>255</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>249</v>
+        <v>256</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>250</v>
+      <c r="D8" s="4" t="s">
+        <v>257</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="F8" s="2">
+      <c r="G8" s="2">
         <v>43853.125</v>
       </c>
-      <c r="G8" s="3">
+      <c r="H8" s="3">
         <v>43859.125</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="4" t="s">
-        <v>251</v>
+        <v>259</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>252</v>
+        <v>260</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>253</v>
+      <c r="D9" s="4" t="s">
+        <v>261</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="F9" s="2">
+      <c r="G9" s="2">
         <v>43892.125</v>
       </c>
-      <c r="G9" s="3">
+      <c r="H9" s="3">
         <v>43924.125</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="s">
-        <v>254</v>
+        <v>263</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>255</v>
+        <v>264</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>256</v>
+      <c r="D10" s="4" t="s">
+        <v>265</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="F10" s="2">
+      <c r="G10" s="2">
         <v>43831.125</v>
       </c>
-      <c r="G10" s="3">
+      <c r="H10" s="3">
         <v>43834.125</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="4" t="s">
-        <v>257</v>
+        <v>267</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>258</v>
+        <v>268</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>259</v>
+      <c r="D11" s="4" t="s">
+        <v>269</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="F11" s="2">
+      <c r="G11" s="2">
         <v>44928.125</v>
       </c>
-      <c r="G11" s="3">
+      <c r="H11" s="3">
         <v>44932.125</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="s">
-        <v>260</v>
+        <v>271</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>261</v>
+        <v>272</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>262</v>
+      <c r="D12" s="4" t="s">
+        <v>273</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="F12" s="2">
+      <c r="G12" s="2">
         <v>45293.125</v>
       </c>
-      <c r="G12" s="3">
+      <c r="H12" s="3">
         <v>45349.125</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="4" t="s">
-        <v>263</v>
+        <v>275</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>264</v>
+        <v>276</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>265</v>
+      <c r="D13" s="4" t="s">
+        <v>277</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="F13" s="2">
+      <c r="G13" s="2">
         <v>44928.125</v>
       </c>
-      <c r="G13" s="3">
+      <c r="H13" s="3">
         <v>44973.125</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="4" t="s">
-        <v>266</v>
+        <v>279</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>267</v>
+        <v>280</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>268</v>
+      <c r="D14" s="4" t="s">
+        <v>281</v>
       </c>
       <c r="E14" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="F14" s="2">
+      <c r="G14" s="2">
         <v>43850.125</v>
       </c>
-      <c r="G14" s="3">
+      <c r="H14" s="3">
         <v>43904.125</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>269</v>
+        <v>283</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>270</v>
+        <v>284</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>271</v>
+      <c r="D15" s="4" t="s">
+        <v>285</v>
       </c>
       <c r="E15" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="F15" s="2">
+      <c r="G15" s="2">
         <v>43853.125</v>
       </c>
-      <c r="G15" s="3">
+      <c r="H15" s="3">
         <v>43856.125</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>272</v>
+        <v>287</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>273</v>
+        <v>288</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>274</v>
+      <c r="D16" s="4" t="s">
+        <v>289</v>
       </c>
       <c r="E16" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="F16" s="2">
-        <v>43832.125</v>
-      </c>
-      <c r="G16" s="3">
+      <c r="G16" s="2">
+        <v>43832.125</v>
+      </c>
+      <c r="H16" s="3">
         <v>43855.125</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>275</v>
+        <v>291</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>276</v>
+        <v>292</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>277</v>
+      <c r="D17" s="4" t="s">
+        <v>293</v>
       </c>
       <c r="E17" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="F17" s="2">
-        <v>43832.125</v>
-      </c>
-      <c r="G17" s="3">
+      <c r="G17" s="2">
+        <v>43832.125</v>
+      </c>
+      <c r="H17" s="3">
         <v>43886.125</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="4" t="s">
-        <v>278</v>
+        <v>295</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>279</v>
+        <v>296</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>280</v>
+      <c r="D18" s="4" t="s">
+        <v>297</v>
       </c>
       <c r="E18" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="F18" s="2">
-        <v>43832.125</v>
-      </c>
-      <c r="G18" s="3">
+      <c r="G18" s="2">
+        <v>43832.125</v>
+      </c>
+      <c r="H18" s="3">
         <v>43866.125</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>281</v>
+        <v>299</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>282</v>
+        <v>300</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>283</v>
+      <c r="D19" s="4" t="s">
+        <v>301</v>
       </c>
       <c r="E19" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="F19" s="2">
-        <v>43832.125</v>
-      </c>
-      <c r="G19" s="3">
+      <c r="G19" s="2">
+        <v>43832.125</v>
+      </c>
+      <c r="H19" s="3">
         <v>43888.125</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="4" t="s">
-        <v>284</v>
+        <v>303</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>285</v>
+        <v>304</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>286</v>
+      <c r="D20" s="4" t="s">
+        <v>305</v>
       </c>
       <c r="E20" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="F20" s="2">
+      <c r="G20" s="2">
         <v>43850.125</v>
       </c>
-      <c r="G20" s="3">
+      <c r="H20" s="3">
         <v>43852.125</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>287</v>
+        <v>307</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>288</v>
+        <v>308</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>289</v>
+      <c r="D21" s="4" t="s">
+        <v>309</v>
       </c>
       <c r="E21" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="F21" s="2">
+      <c r="G21" s="2">
         <v>43853.125</v>
       </c>
-      <c r="G21" s="3">
+      <c r="H21" s="3">
         <v>43887.125</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>290</v>
+        <v>311</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>291</v>
+        <v>312</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>292</v>
+      <c r="D22" s="4" t="s">
+        <v>313</v>
       </c>
       <c r="E22" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="F22" s="2">
+      <c r="G22" s="2">
         <v>43892.125</v>
       </c>
-      <c r="G22" s="3">
+      <c r="H22" s="3">
         <v>43946.125</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>293</v>
+        <v>315</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>294</v>
+        <v>316</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>292</v>
+      <c r="D23" s="4" t="s">
+        <v>317</v>
       </c>
       <c r="E23" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="F23" s="2">
+      <c r="G23" s="2">
         <v>43831.125</v>
       </c>
-      <c r="G23" s="3">
+      <c r="H23" s="3">
         <v>43852.125</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>295</v>
+        <v>318</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>296</v>
+        <v>319</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>297</v>
+      <c r="D24" s="4" t="s">
+        <v>320</v>
       </c>
       <c r="E24" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="F24" s="2">
+      <c r="G24" s="2">
         <v>43853.125</v>
       </c>
-      <c r="G24" s="2">
+      <c r="H24" s="2">
         <v>43887.125</v>
       </c>
     </row>
     <row r="25">
-      <c r="F25" s="2"/>
-      <c r="G25" s="3"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="3"/>
     </row>
     <row r="26">
-      <c r="F26" s="2"/>
-      <c r="G26" s="3"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="3"/>
     </row>
     <row r="27">
-      <c r="F27" s="2"/>
-      <c r="G27" s="3"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="3"/>
     </row>
     <row r="28">
-      <c r="F28" s="2"/>
-      <c r="G28" s="3"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="3"/>
     </row>
     <row r="29">
-      <c r="F29" s="2"/>
-      <c r="G29" s="3"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="3"/>
     </row>
     <row r="30">
-      <c r="F30" s="2"/>
-      <c r="G30" s="3"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="3"/>
     </row>
     <row r="31">
-      <c r="F31" s="2"/>
-      <c r="G31" s="3"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="3"/>
     </row>
     <row r="32">
-      <c r="F32" s="2"/>
-      <c r="G32" s="3"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="3"/>
     </row>
     <row r="33">
-      <c r="F33" s="2"/>
-      <c r="G33" s="3"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="3"/>
     </row>
     <row r="34">
-      <c r="F34" s="2"/>
-      <c r="G34" s="3"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="3"/>
     </row>
     <row r="35">
-      <c r="F35" s="2"/>
-      <c r="G35" s="3"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="3"/>
     </row>
     <row r="36">
-      <c r="F36" s="2"/>
-      <c r="G36" s="3"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="3"/>
     </row>
     <row r="37">
-      <c r="F37" s="2"/>
-      <c r="G37" s="3"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="3"/>
     </row>
     <row r="38">
-      <c r="F38" s="2"/>
-      <c r="G38" s="3"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="3"/>
     </row>
     <row r="39">
-      <c r="F39" s="2"/>
-      <c r="G39" s="3"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="3"/>
     </row>
     <row r="40">
-      <c r="F40" s="2"/>
-      <c r="G40" s="3"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="3"/>
     </row>
     <row r="41">
-      <c r="F41" s="2"/>
-      <c r="G41" s="3"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="3"/>
     </row>
     <row r="42">
-      <c r="F42" s="2"/>
-      <c r="G42" s="3"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="3"/>
     </row>
     <row r="43">
-      <c r="F43" s="2"/>
-      <c r="G43" s="3"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="3"/>
     </row>
     <row r="44">
-      <c r="F44" s="2"/>
-      <c r="G44" s="3"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="3"/>
     </row>
     <row r="45">
-      <c r="F45" s="2"/>
-      <c r="G45" s="3"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="3"/>
     </row>
     <row r="46">
-      <c r="F46" s="2"/>
-      <c r="G46" s="3"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="3"/>
     </row>
     <row r="47">
-      <c r="F47" s="2"/>
-      <c r="G47" s="3"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="3"/>
     </row>
     <row r="48">
-      <c r="F48" s="2"/>
-      <c r="G48" s="3"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="3"/>
     </row>
     <row r="49">
-      <c r="F49" s="2"/>
-      <c r="G49" s="3"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="3"/>
     </row>
     <row r="50">
-      <c r="F50" s="2"/>
-      <c r="G50" s="3"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="3"/>
     </row>
     <row r="51">
-      <c r="F51" s="2"/>
-      <c r="G51" s="3"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="3"/>
     </row>
     <row r="52">
-      <c r="F52" s="2"/>
-      <c r="G52" s="3"/>
+      <c r="G52" s="2"/>
+      <c r="H52" s="3"/>
     </row>
     <row r="53">
-      <c r="F53" s="2"/>
-      <c r="G53" s="3"/>
+      <c r="G53" s="2"/>
+      <c r="H53" s="3"/>
     </row>
     <row r="54">
-      <c r="F54" s="2"/>
-      <c r="G54" s="3"/>
+      <c r="G54" s="2"/>
+      <c r="H54" s="3"/>
     </row>
     <row r="55">
-      <c r="F55" s="2"/>
-      <c r="G55" s="3"/>
+      <c r="G55" s="2"/>
+      <c r="H55" s="3"/>
     </row>
     <row r="56">
-      <c r="F56" s="2"/>
-      <c r="G56" s="3"/>
+      <c r="G56" s="2"/>
+      <c r="H56" s="3"/>
     </row>
     <row r="57">
-      <c r="F57" s="2"/>
-      <c r="G57" s="3"/>
+      <c r="G57" s="2"/>
+      <c r="H57" s="3"/>
     </row>
     <row r="58">
-      <c r="F58" s="2"/>
-      <c r="G58" s="3"/>
+      <c r="G58" s="2"/>
+      <c r="H58" s="3"/>
     </row>
     <row r="59">
-      <c r="F59" s="2"/>
-      <c r="G59" s="3"/>
+      <c r="G59" s="2"/>
+      <c r="H59" s="3"/>
     </row>
     <row r="60">
-      <c r="F60" s="2"/>
-      <c r="G60" s="3"/>
+      <c r="G60" s="2"/>
+      <c r="H60" s="3"/>
     </row>
     <row r="61">
-      <c r="F61" s="2"/>
-      <c r="G61" s="3"/>
+      <c r="G61" s="2"/>
+      <c r="H61" s="3"/>
     </row>
     <row r="62">
-      <c r="F62" s="2"/>
-      <c r="G62" s="3"/>
+      <c r="G62" s="2"/>
+      <c r="H62" s="3"/>
     </row>
     <row r="63">
-      <c r="F63" s="2"/>
-      <c r="G63" s="3"/>
+      <c r="G63" s="2"/>
+      <c r="H63" s="3"/>
     </row>
     <row r="64">
-      <c r="F64" s="2"/>
-      <c r="G64" s="3"/>
+      <c r="G64" s="2"/>
+      <c r="H64" s="3"/>
     </row>
     <row r="65">
-      <c r="F65" s="2"/>
-      <c r="G65" s="3"/>
+      <c r="G65" s="2"/>
+      <c r="H65" s="3"/>
     </row>
     <row r="66">
-      <c r="F66" s="2"/>
-      <c r="G66" s="3"/>
+      <c r="G66" s="2"/>
+      <c r="H66" s="3"/>
     </row>
     <row r="67">
-      <c r="F67" s="2"/>
-      <c r="G67" s="3"/>
+      <c r="G67" s="2"/>
+      <c r="H67" s="3"/>
     </row>
     <row r="68">
-      <c r="F68" s="2"/>
-      <c r="G68" s="3"/>
+      <c r="G68" s="2"/>
+      <c r="H68" s="3"/>
     </row>
     <row r="69">
-      <c r="F69" s="2"/>
-      <c r="G69" s="3"/>
+      <c r="G69" s="2"/>
+      <c r="H69" s="3"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -3763,9 +4043,9 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="23.38"/>
-    <col customWidth="1" min="2" max="2" width="119.38"/>
-    <col customWidth="1" min="5" max="5" width="16.13"/>
+    <col customWidth="1" min="1" max="2" width="23.38"/>
+    <col customWidth="1" min="3" max="3" width="119.38"/>
+    <col customWidth="1" min="6" max="6" width="16.13"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3773,996 +4053,1131 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>298</v>
+        <v>322</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>300</v>
+        <v>324</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>230</v>
+        <v>326</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="C2" s="1">
+        <v>231</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="D2" s="1">
         <v>4.0</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="5">
-        <v>43832.125</v>
-      </c>
-      <c r="F2" s="3">
+      <c r="F2" s="5">
+        <v>43832.125</v>
+      </c>
+      <c r="G2" s="3">
         <v>43834.125</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="s">
-        <v>233</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="C3" s="1">
+      <c r="A3" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="D3" s="1">
         <v>5.0</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="5">
-        <v>43832.125</v>
-      </c>
-      <c r="F3" s="3">
+      <c r="F3" s="5">
+        <v>43832.125</v>
+      </c>
+      <c r="G3" s="3">
         <v>43835.125</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="s">
-        <v>236</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="C4" s="1">
+      <c r="A4" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="D4" s="1">
         <v>3.0</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="5">
-        <v>43832.125</v>
-      </c>
-      <c r="F4" s="3">
+      <c r="F4" s="5">
+        <v>43832.125</v>
+      </c>
+      <c r="G4" s="3">
         <v>43875.125</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>239</v>
+        <v>332</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="C5" s="1">
+        <v>243</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="D5" s="1">
         <v>4.0</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E5" s="5">
-        <v>43832.125</v>
-      </c>
-      <c r="F5" s="3">
+      <c r="F5" s="5">
+        <v>43832.125</v>
+      </c>
+      <c r="G5" s="3">
         <v>43837.125</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>242</v>
+        <v>334</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="C6" s="1">
+        <v>247</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="D6" s="1">
         <v>5.0</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="5">
-        <v>43832.125</v>
-      </c>
-      <c r="F6" s="3">
+      <c r="F6" s="5">
+        <v>43832.125</v>
+      </c>
+      <c r="G6" s="3">
         <v>43875.125</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="C7" s="1">
+      <c r="A7" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="D7" s="1">
         <v>5.0</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="5">
+      <c r="F7" s="5">
         <v>43850.125</v>
       </c>
-      <c r="F7" s="3">
+      <c r="G7" s="3">
         <v>43895.125</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="4" t="s">
-        <v>248</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="C8" s="1">
+      <c r="A8" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="D8" s="1">
         <v>4.0</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="5">
+      <c r="F8" s="5">
         <v>43853.125</v>
       </c>
-      <c r="F8" s="3">
+      <c r="G8" s="3">
         <v>43859.125</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="4" t="s">
-        <v>251</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="C9" s="1">
+      <c r="A9" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="D9" s="1">
         <v>3.0</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E9" s="5">
+      <c r="F9" s="5">
         <v>43892.125</v>
       </c>
-      <c r="F9" s="3">
+      <c r="G9" s="3">
         <v>43924.125</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="4" t="s">
-        <v>254</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="C10" s="1">
+      <c r="A10" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="D10" s="1">
         <v>4.0</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E10" s="5">
+      <c r="F10" s="5">
         <v>43831.125</v>
       </c>
-      <c r="F10" s="3">
+      <c r="G10" s="3">
         <v>43834.125</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="C11" s="1">
+      <c r="A11" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="D11" s="1">
         <v>4.0</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E11" s="5">
+      <c r="F11" s="5">
         <v>44928.125</v>
       </c>
-      <c r="F11" s="3">
+      <c r="G11" s="3">
         <v>44932.125</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="4" t="s">
-        <v>260</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="C12" s="1">
+      <c r="A12" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="D12" s="1">
         <v>4.0</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E12" s="5">
+      <c r="F12" s="5">
         <v>45293.125</v>
       </c>
-      <c r="F12" s="3">
+      <c r="G12" s="3">
         <v>45349.125</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="4" t="s">
-        <v>263</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="C13" s="1">
+      <c r="A13" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="D13" s="1">
         <v>5.0</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E13" s="5">
+      <c r="F13" s="5">
         <v>44928.125</v>
       </c>
-      <c r="F13" s="3">
+      <c r="G13" s="3">
         <v>44973.125</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="4" t="s">
-        <v>266</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="C14" s="1">
+      <c r="A14" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="D14" s="1">
         <v>5.0</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E14" s="5">
+      <c r="F14" s="5">
         <v>43850.125</v>
       </c>
-      <c r="F14" s="3">
+      <c r="G14" s="3">
         <v>43904.125</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>314</v>
+        <v>352</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="C15" s="1">
+        <v>353</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="D15" s="1">
         <v>4.0</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E15" s="5">
+      <c r="F15" s="5">
         <v>43853.125</v>
       </c>
-      <c r="F15" s="3">
+      <c r="G15" s="3">
         <v>43856.125</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>272</v>
+        <v>355</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="C16" s="1">
+        <v>287</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="D16" s="1">
         <v>4.0</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E16" s="5">
-        <v>43832.125</v>
-      </c>
-      <c r="F16" s="3">
+      <c r="F16" s="5">
+        <v>43832.125</v>
+      </c>
+      <c r="G16" s="3">
         <v>43855.125</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>275</v>
+        <v>357</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="C17" s="1">
+        <v>291</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="D17" s="1">
         <v>5.0</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E17" s="5">
-        <v>43832.125</v>
-      </c>
-      <c r="F17" s="3">
+      <c r="F17" s="5">
+        <v>43832.125</v>
+      </c>
+      <c r="G17" s="3">
         <v>43886.125</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="C18" s="1">
+      <c r="A18" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="D18" s="1">
         <v>3.0</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E18" s="5">
-        <v>43832.125</v>
-      </c>
-      <c r="F18" s="3">
+      <c r="F18" s="5">
+        <v>43832.125</v>
+      </c>
+      <c r="G18" s="3">
         <v>43866.125</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>281</v>
+        <v>361</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="C19" s="1">
+        <v>299</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="D19" s="1">
         <v>4.0</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E19" s="5">
-        <v>43832.125</v>
-      </c>
-      <c r="F19" s="3">
+      <c r="F19" s="5">
+        <v>43832.125</v>
+      </c>
+      <c r="G19" s="3">
         <v>43888.125</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="4" t="s">
-        <v>284</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="C20" s="1">
+      <c r="A20" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="D20" s="1">
         <v>4.0</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E20" s="5">
+      <c r="F20" s="5">
         <v>43850.125</v>
       </c>
-      <c r="F20" s="3">
+      <c r="G20" s="3">
         <v>43852.125</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="4" t="s">
-        <v>321</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="C21" s="1">
+      <c r="A21" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="D21" s="1">
         <v>4.0</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E21" s="5">
+      <c r="F21" s="5">
         <v>43853.125</v>
       </c>
-      <c r="F21" s="3">
+      <c r="G21" s="3">
         <v>43887.125</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>290</v>
+        <v>368</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="C22" s="1">
+        <v>311</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="D22" s="1">
         <v>5.0</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="E22" s="5">
+      <c r="F22" s="5">
         <v>43892.125</v>
       </c>
-      <c r="F22" s="3">
+      <c r="G22" s="3">
         <v>43946.125</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="4" t="s">
-        <v>324</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="C23" s="1">
+      <c r="A23" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="D23" s="1">
         <v>5.0</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="E23" s="5">
+      <c r="F23" s="5">
         <v>43831.125</v>
       </c>
-      <c r="F23" s="3">
+      <c r="G23" s="3">
         <v>43852.125</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>230</v>
+        <v>373</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="C24" s="1">
+        <v>231</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="D24" s="1">
         <v>5.0</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="E24" s="5">
+      <c r="F24" s="5">
         <v>44928.125</v>
       </c>
-      <c r="F24" s="3">
+      <c r="G24" s="3">
         <v>44962.125</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="4" t="s">
-        <v>233</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="C25" s="1">
+      <c r="A25" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="D25" s="1">
         <v>5.0</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E25" s="5">
+      <c r="F25" s="5">
         <v>45293.125</v>
       </c>
-      <c r="F25" s="3">
+      <c r="G25" s="3">
         <v>45349.125</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="4" t="s">
-        <v>236</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="C26" s="1">
+      <c r="A26" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="D26" s="1">
         <v>4.0</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E26" s="5">
-        <v>43832.125</v>
-      </c>
-      <c r="F26" s="3">
+      <c r="F26" s="5">
+        <v>43832.125</v>
+      </c>
+      <c r="G26" s="3">
         <v>43839.125</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>239</v>
+        <v>379</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="C27" s="1">
+        <v>243</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="D27" s="1">
         <v>5.0</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E27" s="5">
-        <v>43832.125</v>
-      </c>
-      <c r="F27" s="3">
+      <c r="F27" s="5">
+        <v>43832.125</v>
+      </c>
+      <c r="G27" s="3">
         <v>43886.125</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>242</v>
+        <v>381</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="C28" s="1">
+        <v>247</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="D28" s="1">
         <v>5.0</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="E28" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E28" s="5">
-        <v>43832.125</v>
-      </c>
-      <c r="F28" s="3">
+      <c r="F28" s="5">
+        <v>43832.125</v>
+      </c>
+      <c r="G28" s="3">
         <v>43910.125</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>331</v>
-      </c>
-      <c r="C29" s="1">
+      <c r="A29" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="D29" s="1">
         <v>5.0</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="E29" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="E29" s="5">
+      <c r="F29" s="5">
         <v>43850.125</v>
       </c>
-      <c r="F29" s="3">
+      <c r="G29" s="3">
         <v>43859.125</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="4" t="s">
-        <v>248</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="C30" s="1">
+      <c r="A30" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="D30" s="1">
         <v>4.0</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="E30" s="5">
+      <c r="F30" s="5">
         <v>43853.125</v>
       </c>
-      <c r="F30" s="3">
+      <c r="G30" s="3">
         <v>43861.125</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="4" t="s">
-        <v>251</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C31" s="1">
+      <c r="A31" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="D31" s="1">
         <v>3.0</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="E31" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="E31" s="5">
+      <c r="F31" s="5">
         <v>43892.125</v>
       </c>
-      <c r="F31" s="3">
+      <c r="G31" s="3">
         <v>43899.125</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="4" t="s">
-        <v>254</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>334</v>
-      </c>
-      <c r="C32" s="1">
+      <c r="A32" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="D32" s="1">
         <v>4.0</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="E32" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E32" s="5">
+      <c r="F32" s="5">
         <v>43831.125</v>
       </c>
-      <c r="F32" s="3">
+      <c r="G32" s="3">
         <v>43865.125</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="C33" s="1">
+      <c r="A33" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="D33" s="1">
         <v>4.0</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="E33" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="E33" s="5">
+      <c r="F33" s="5">
         <v>44928.125</v>
       </c>
-      <c r="F33" s="3">
+      <c r="G33" s="3">
         <v>44981.125</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="4" t="s">
-        <v>260</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="C34" s="1">
+      <c r="A34" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="D34" s="1">
         <v>5.0</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="E34" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="E34" s="5">
+      <c r="F34" s="5">
         <v>45293.125</v>
       </c>
-      <c r="F34" s="3">
+      <c r="G34" s="3">
         <v>45295.125</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="4" t="s">
-        <v>263</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="C35" s="1">
+      <c r="A35" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="D35" s="1">
         <v>5.0</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="E35" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E35" s="5">
-        <v>43832.125</v>
-      </c>
-      <c r="F35" s="3">
+      <c r="F35" s="5">
+        <v>43832.125</v>
+      </c>
+      <c r="G35" s="3">
         <v>43844.125</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="4" t="s">
-        <v>266</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="C36" s="1">
+      <c r="A36" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="D36" s="1">
         <v>4.0</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="E36" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E36" s="5">
-        <v>43832.125</v>
-      </c>
-      <c r="F36" s="3">
+      <c r="F36" s="5">
+        <v>43832.125</v>
+      </c>
+      <c r="G36" s="3">
         <v>43837.125</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>314</v>
+        <v>399</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="C37" s="1">
+        <v>353</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="D37" s="1">
         <v>5.0</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="E37" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E37" s="5">
-        <v>43832.125</v>
-      </c>
-      <c r="F37" s="3">
+      <c r="F37" s="5">
+        <v>43832.125</v>
+      </c>
+      <c r="G37" s="3">
         <v>43919.125</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>272</v>
+        <v>401</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="C38" s="1">
+        <v>287</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="D38" s="1">
         <v>4.0</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="E38" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E38" s="5">
-        <v>43832.125</v>
-      </c>
-      <c r="F38" s="3">
+      <c r="F38" s="5">
+        <v>43832.125</v>
+      </c>
+      <c r="G38" s="3">
         <v>43897.125</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>275</v>
+        <v>403</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="C39" s="1">
+        <v>291</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="D39" s="1">
         <v>4.0</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="E39" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="E39" s="5">
+      <c r="F39" s="5">
         <v>43850.125</v>
       </c>
-      <c r="F39" s="3">
+      <c r="G39" s="3">
         <v>43893.125</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="C40" s="1">
+      <c r="A40" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="D40" s="1">
         <v>5.0</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="E40" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E40" s="5">
+      <c r="F40" s="5">
         <v>43853.125</v>
       </c>
-      <c r="F40" s="3">
+      <c r="G40" s="3">
         <v>43876.125</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>281</v>
+        <v>407</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="C41" s="1">
+        <v>299</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="D41" s="1">
         <v>4.0</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="E41" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E41" s="5">
+      <c r="F41" s="5">
         <v>43892.125</v>
       </c>
-      <c r="F41" s="3">
+      <c r="G41" s="3">
         <v>43937.125</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="4" t="s">
-        <v>284</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>344</v>
-      </c>
-      <c r="C42" s="1">
+      <c r="A42" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="D42" s="1">
         <v>5.0</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="E42" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E42" s="5">
+      <c r="F42" s="5">
         <v>43831.125</v>
       </c>
-      <c r="F42" s="3">
+      <c r="G42" s="3">
         <v>43907.125</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="4" t="s">
-        <v>321</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>345</v>
-      </c>
-      <c r="C43" s="1">
+      <c r="A43" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="D43" s="1">
         <v>3.0</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="E43" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="E43" s="5">
+      <c r="F43" s="5">
         <v>44928.125</v>
       </c>
-      <c r="F43" s="3">
+      <c r="G43" s="3">
         <v>44982.125</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>290</v>
+        <v>413</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>346</v>
-      </c>
-      <c r="C44" s="1">
+        <v>311</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="D44" s="1">
         <v>4.0</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="E44" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E44" s="5">
+      <c r="F44" s="5">
         <v>45293.125</v>
       </c>
-      <c r="F44" s="3">
+      <c r="G44" s="3">
         <v>45360.125</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="4" t="s">
-        <v>324</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>347</v>
-      </c>
-      <c r="C45" s="1">
+      <c r="A45" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="D45" s="1">
         <v>5.0</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="E45" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E45" s="5">
+      <c r="F45" s="5">
         <v>45293.125</v>
       </c>
-      <c r="F45" s="3">
+      <c r="G45" s="3">
         <v>45373.125</v>
       </c>
     </row>
     <row r="46">
-      <c r="E46" s="5"/>
-      <c r="F46" s="3"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="3"/>
     </row>
     <row r="47">
-      <c r="E47" s="2"/>
-      <c r="F47" s="3"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="3"/>
     </row>
     <row r="48">
-      <c r="E48" s="2"/>
-      <c r="F48" s="3"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="3"/>
     </row>
     <row r="49">
-      <c r="E49" s="2"/>
-      <c r="F49" s="3"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="3"/>
     </row>
     <row r="50">
-      <c r="E50" s="2"/>
-      <c r="F50" s="3"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="3"/>
     </row>
     <row r="51">
-      <c r="E51" s="2"/>
-      <c r="F51" s="3"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="3"/>
     </row>
     <row r="52">
-      <c r="E52" s="2"/>
-      <c r="F52" s="3"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="3"/>
     </row>
     <row r="53">
-      <c r="E53" s="2"/>
-      <c r="F53" s="3"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="3"/>
     </row>
     <row r="54">
-      <c r="E54" s="2"/>
-      <c r="F54" s="3"/>
+      <c r="F54" s="2"/>
+      <c r="G54" s="3"/>
     </row>
     <row r="55">
-      <c r="E55" s="2"/>
-      <c r="F55" s="3"/>
+      <c r="F55" s="2"/>
+      <c r="G55" s="3"/>
     </row>
     <row r="56">
-      <c r="E56" s="2"/>
-      <c r="F56" s="3"/>
+      <c r="F56" s="2"/>
+      <c r="G56" s="3"/>
     </row>
     <row r="57">
-      <c r="E57" s="2"/>
-      <c r="F57" s="3"/>
+      <c r="F57" s="2"/>
+      <c r="G57" s="3"/>
     </row>
     <row r="58">
-      <c r="E58" s="2"/>
-      <c r="F58" s="3"/>
+      <c r="F58" s="2"/>
+      <c r="G58" s="3"/>
     </row>
     <row r="59">
-      <c r="E59" s="2"/>
-      <c r="F59" s="3"/>
+      <c r="F59" s="2"/>
+      <c r="G59" s="3"/>
     </row>
     <row r="60">
-      <c r="E60" s="2"/>
-      <c r="F60" s="3"/>
+      <c r="F60" s="2"/>
+      <c r="G60" s="3"/>
     </row>
     <row r="61">
-      <c r="E61" s="2"/>
-      <c r="F61" s="3"/>
+      <c r="F61" s="2"/>
+      <c r="G61" s="3"/>
     </row>
     <row r="62">
-      <c r="E62" s="2"/>
-      <c r="F62" s="3"/>
+      <c r="F62" s="2"/>
+      <c r="G62" s="3"/>
     </row>
     <row r="63">
-      <c r="E63" s="2"/>
-      <c r="F63" s="3"/>
+      <c r="F63" s="2"/>
+      <c r="G63" s="3"/>
     </row>
     <row r="64">
-      <c r="E64" s="2"/>
-      <c r="F64" s="3"/>
+      <c r="F64" s="2"/>
+      <c r="G64" s="3"/>
     </row>
     <row r="65">
-      <c r="E65" s="2"/>
-      <c r="F65" s="3"/>
+      <c r="F65" s="2"/>
+      <c r="G65" s="3"/>
     </row>
     <row r="66">
-      <c r="E66" s="2"/>
-      <c r="F66" s="3"/>
+      <c r="F66" s="2"/>
+      <c r="G66" s="3"/>
     </row>
     <row r="67">
-      <c r="E67" s="2"/>
-      <c r="F67" s="3"/>
+      <c r="F67" s="2"/>
+      <c r="G67" s="3"/>
     </row>
     <row r="68">
-      <c r="E68" s="2"/>
-      <c r="F68" s="3"/>
+      <c r="F68" s="2"/>
+      <c r="G68" s="3"/>
     </row>
     <row r="69">
-      <c r="E69" s="2"/>
-      <c r="F69" s="3"/>
+      <c r="F69" s="2"/>
+      <c r="G69" s="3"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -4789,7 +5204,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>348</v>
+        <v>417</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -4803,13 +5218,13 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>349</v>
+        <v>418</v>
       </c>
       <c r="B2" s="1">
         <v>4.0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>350</v>
+        <v>419</v>
       </c>
       <c r="D2" s="2">
         <v>43832.125</v>
@@ -4820,13 +5235,13 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>351</v>
+        <v>420</v>
       </c>
       <c r="B3" s="1">
         <v>3.0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>352</v>
+        <v>421</v>
       </c>
       <c r="D3" s="2">
         <v>43832.125</v>
@@ -4837,13 +5252,13 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>353</v>
+        <v>422</v>
       </c>
       <c r="B4" s="1">
         <v>2.0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>354</v>
+        <v>423</v>
       </c>
       <c r="D4" s="2">
         <v>43832.125</v>
@@ -4854,13 +5269,13 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>355</v>
+        <v>424</v>
       </c>
       <c r="B5" s="1">
         <v>1.0</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>356</v>
+        <v>425</v>
       </c>
       <c r="D5" s="2">
         <v>43832.125</v>

</xml_diff>

<commit_message>
fixed: OpenAPI + swagger docs
</commit_message>
<xml_diff>
--- a/seeds/seeds.xlsx
+++ b/seeds/seeds.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="430">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="427">
   <si>
     <t>id</t>
   </si>
@@ -1115,9 +1115,6 @@
     <t>uuid-review-14</t>
   </si>
   <si>
-    <t>uuid-patinaço</t>
-  </si>
-  <si>
     <t>A pista de patinação é ampla e bem cuidada. Um lugar divertido para famílias e amigos. Eles também oferecem aulas para iniciantes</t>
   </si>
   <si>
@@ -1154,9 +1151,6 @@
     <t>uuid-review-20</t>
   </si>
   <si>
-    <t>uuid-piscinão-azul</t>
-  </si>
-  <si>
     <t>A melhor fuga do calor! O parque aquático tem opções para todos, desde piscinas tranquilas até escorregadores emocionantes.</t>
   </si>
   <si>
@@ -1167,9 +1161,6 @@
   </si>
   <si>
     <t>uuid-review-22</t>
-  </si>
-  <si>
-    <t>uuid-pizzarolla</t>
   </si>
   <si>
     <t>Uma pizzaria que se destaca. A massa fina e crocante e os ingredientes frescos fazem toda a diferença. Excelente atendimento também</t>
@@ -8648,10 +8639,10 @@
         <v>365</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>366</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>367</v>
       </c>
       <c r="D15" s="1">
         <v>4.0</v>
@@ -8668,13 +8659,13 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>300</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D16" s="1">
         <v>4.0</v>
@@ -8691,13 +8682,13 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>304</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D17" s="1">
         <v>5.0</v>
@@ -8714,13 +8705,13 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>308</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D18" s="1">
         <v>3.0</v>
@@ -8737,13 +8728,13 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>312</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D19" s="1">
         <v>4.0</v>
@@ -8760,13 +8751,13 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>316</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D20" s="1">
         <v>4.0</v>
@@ -8783,13 +8774,13 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>378</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>379</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>380</v>
       </c>
       <c r="D21" s="1">
         <v>4.0</v>
@@ -8806,13 +8797,13 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>324</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="D22" s="1">
         <v>5.0</v>
@@ -8829,13 +8820,13 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>383</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>384</v>
+        <v>381</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>328</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D23" s="1">
         <v>5.0</v>
@@ -8852,13 +8843,13 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>244</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D24" s="1">
         <v>5.0</v>
@@ -8875,13 +8866,13 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>248</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="D25" s="1">
         <v>5.0</v>
@@ -8898,13 +8889,13 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>252</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="D26" s="1">
         <v>4.0</v>
@@ -8921,13 +8912,13 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>256</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="D27" s="1">
         <v>5.0</v>
@@ -8944,13 +8935,13 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>260</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="D28" s="1">
         <v>5.0</v>
@@ -8967,13 +8958,13 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>264</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="D29" s="1">
         <v>5.0</v>
@@ -8990,13 +8981,13 @@
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>268</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="D30" s="1">
         <v>4.0</v>
@@ -9013,13 +9004,13 @@
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>272</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="D31" s="1">
         <v>3.0</v>
@@ -9036,13 +9027,13 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>276</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D32" s="1">
         <v>4.0</v>
@@ -9059,13 +9050,13 @@
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>280</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="D33" s="1">
         <v>4.0</v>
@@ -9082,13 +9073,13 @@
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>284</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="D34" s="1">
         <v>5.0</v>
@@ -9105,13 +9096,13 @@
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B35" s="6" t="s">
         <v>288</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="D35" s="1">
         <v>5.0</v>
@@ -9128,13 +9119,13 @@
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>292</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="D36" s="1">
         <v>4.0</v>
@@ -9151,13 +9142,13 @@
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>366</v>
+        <v>296</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="D37" s="1">
         <v>5.0</v>
@@ -9174,13 +9165,13 @@
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>300</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="D38" s="1">
         <v>4.0</v>
@@ -9197,13 +9188,13 @@
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>304</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="D39" s="1">
         <v>4.0</v>
@@ -9220,13 +9211,13 @@
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="B40" s="6" t="s">
         <v>308</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="D40" s="1">
         <v>5.0</v>
@@ -9243,13 +9234,13 @@
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>312</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="D41" s="1">
         <v>4.0</v>
@@ -9266,13 +9257,13 @@
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="B42" s="6" t="s">
         <v>316</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="D42" s="1">
         <v>5.0</v>
@@ -9289,13 +9280,13 @@
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>424</v>
-      </c>
-      <c r="B43" s="6" t="s">
-        <v>379</v>
+        <v>421</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>320</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="D43" s="1">
         <v>3.0</v>
@@ -9312,13 +9303,13 @@
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>324</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="D44" s="1">
         <v>4.0</v>
@@ -9335,13 +9326,13 @@
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>428</v>
-      </c>
-      <c r="B45" s="6" t="s">
-        <v>384</v>
+        <v>425</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>328</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="D45" s="1">
         <v>5.0</v>

</xml_diff>